<commit_message>
Tweaks to baseline data
having found better sources. Willeke has module MFG eff at 98% in 2002, so set all years equal to 98% for now.
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/SupportingMaterial/BaselineGraphs.xlsx
+++ b/PV_ICE/baselines/SupportingMaterial/BaselineGraphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A3D3A5-D1A7-451D-98E2-D9735D6E3CBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58748E4A-488F-4EFA-AF6E-079DCECF6256}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-2340" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{31D47E9D-A833-4D35-B79A-EFF0E4DE6D01}"/>
   </bookViews>
@@ -1064,130 +1064,130 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="42"/>
                 <c:pt idx="0">
-                  <c:v>77</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>78</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>78</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>79</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>79</c:v>
+                  <c:v>95.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>80</c:v>
+                  <c:v>95.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>81</c:v>
+                  <c:v>95.7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>82</c:v>
+                  <c:v>95.9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>82</c:v>
+                  <c:v>96.2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>82</c:v>
+                  <c:v>96.4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>83</c:v>
+                  <c:v>96.6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>83</c:v>
+                  <c:v>96.9</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>83</c:v>
+                  <c:v>97.1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>83</c:v>
+                  <c:v>97.4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>83</c:v>
+                  <c:v>97.6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>83</c:v>
+                  <c:v>97.8</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>83</c:v>
+                  <c:v>98.1</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>83</c:v>
+                  <c:v>98.3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>83</c:v>
+                  <c:v>98.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>83</c:v>
+                  <c:v>98.8</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5164,172 +5164,172 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
                 <c:pt idx="0">
-                  <c:v>74.599999999999994</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>74.599999999999994</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>74.599999999999994</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>74.599999999999994</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>74.599999999999994</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>75</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>75</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>75</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>75</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>76</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>76</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>76</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>77</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>77</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>77</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>78</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>78</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>78</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>79</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>79</c:v>
+                  <c:v>95.2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>80</c:v>
+                  <c:v>95.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>81</c:v>
+                  <c:v>95.7</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>82</c:v>
+                  <c:v>95.9</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>82</c:v>
+                  <c:v>96.2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>82</c:v>
+                  <c:v>96.4</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>83</c:v>
+                  <c:v>96.6</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>83</c:v>
+                  <c:v>96.9</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>83</c:v>
+                  <c:v>97.1</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>83</c:v>
+                  <c:v>97.4</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>83</c:v>
+                  <c:v>97.6</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>83</c:v>
+                  <c:v>97.8</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>83</c:v>
+                  <c:v>98.1</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>83</c:v>
+                  <c:v>98.3</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>83</c:v>
+                  <c:v>98.5</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>83</c:v>
+                  <c:v>98.8</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>83</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -26298,16 +26298,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>274637</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>382587</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>106360</xdr:rowOff>
+      <xdr:rowOff>131760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>311150</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -32840,7 +32840,7 @@
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -32870,7 +32870,7 @@
         <v>1995</v>
       </c>
       <c r="B2">
-        <v>74.599999999999994</v>
+        <v>95</v>
       </c>
       <c r="C2">
         <v>50</v>
@@ -32890,7 +32890,7 @@
         <v>1996</v>
       </c>
       <c r="B3">
-        <v>74.599999999999994</v>
+        <v>95</v>
       </c>
       <c r="C3">
         <v>50</v>
@@ -32910,7 +32910,7 @@
         <v>1997</v>
       </c>
       <c r="B4">
-        <v>74.599999999999994</v>
+        <v>95</v>
       </c>
       <c r="C4">
         <v>50</v>
@@ -32930,7 +32930,7 @@
         <v>1998</v>
       </c>
       <c r="B5">
-        <v>74.599999999999994</v>
+        <v>95</v>
       </c>
       <c r="C5">
         <v>50</v>
@@ -32950,7 +32950,7 @@
         <v>1999</v>
       </c>
       <c r="B6">
-        <v>74.599999999999994</v>
+        <v>95</v>
       </c>
       <c r="C6">
         <v>50</v>
@@ -32970,7 +32970,7 @@
         <v>2000</v>
       </c>
       <c r="B7">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="C7">
         <v>50</v>
@@ -32990,7 +32990,7 @@
         <v>2001</v>
       </c>
       <c r="B8">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="C8">
         <v>50</v>
@@ -33010,7 +33010,7 @@
         <v>2002</v>
       </c>
       <c r="B9">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="C9">
         <v>50</v>
@@ -33030,7 +33030,7 @@
         <v>2003</v>
       </c>
       <c r="B10">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="C10">
         <v>50</v>
@@ -33050,7 +33050,7 @@
         <v>2004</v>
       </c>
       <c r="B11">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="C11">
         <v>49.365658340000003</v>
@@ -33070,7 +33070,7 @@
         <v>2005</v>
       </c>
       <c r="B12">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="C12">
         <v>41.588057310000003</v>
@@ -33090,7 +33090,7 @@
         <v>2006</v>
       </c>
       <c r="B13">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="C13">
         <v>33.638416139999997</v>
@@ -33110,7 +33110,7 @@
         <v>2007</v>
       </c>
       <c r="B14">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="C14">
         <v>32.313886099999998</v>
@@ -33130,7 +33130,7 @@
         <v>2008</v>
       </c>
       <c r="B15">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="C15">
         <v>30.95939478</v>
@@ -33150,7 +33150,7 @@
         <v>2009</v>
       </c>
       <c r="B16">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="C16">
         <v>31.313555950000001</v>
@@ -33170,7 +33170,7 @@
         <v>2010</v>
       </c>
       <c r="B17">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="C17">
         <v>49.33536239</v>
@@ -33190,7 +33190,7 @@
         <v>2011</v>
       </c>
       <c r="B18">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="C18">
         <v>49.661818310000001</v>
@@ -33210,7 +33210,7 @@
         <v>2012</v>
       </c>
       <c r="B19">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="C19">
         <v>48.63711241</v>
@@ -33230,7 +33230,7 @@
         <v>2013</v>
       </c>
       <c r="B20">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="C20">
         <v>49.920500959999998</v>
@@ -33250,7 +33250,7 @@
         <v>2014</v>
       </c>
       <c r="B21">
-        <v>79</v>
+        <v>95.2</v>
       </c>
       <c r="C21">
         <v>50.133176429999999</v>
@@ -33270,7 +33270,7 @@
         <v>2015</v>
       </c>
       <c r="B22">
-        <v>80</v>
+        <v>95.5</v>
       </c>
       <c r="C22">
         <v>50.540356459999998</v>
@@ -33290,7 +33290,7 @@
         <v>2016</v>
       </c>
       <c r="B23">
-        <v>81</v>
+        <v>95.7</v>
       </c>
       <c r="C23">
         <v>53.417000399999999</v>
@@ -33310,7 +33310,7 @@
         <v>2017</v>
       </c>
       <c r="B24">
-        <v>82</v>
+        <v>95.9</v>
       </c>
       <c r="C24">
         <v>59.32333715</v>
@@ -33330,7 +33330,7 @@
         <v>2018</v>
       </c>
       <c r="B25">
-        <v>82</v>
+        <v>96.2</v>
       </c>
       <c r="C25">
         <v>63.600552669999999</v>
@@ -33350,7 +33350,7 @@
         <v>2019</v>
       </c>
       <c r="B26">
-        <v>82</v>
+        <v>96.4</v>
       </c>
       <c r="C26">
         <v>65.063940110000004</v>
@@ -33370,7 +33370,7 @@
         <v>2020</v>
       </c>
       <c r="B27">
-        <v>83</v>
+        <v>96.6</v>
       </c>
       <c r="C27">
         <v>66.726759759999993</v>
@@ -33390,7 +33390,7 @@
         <v>2021</v>
       </c>
       <c r="B28">
-        <v>83</v>
+        <v>96.9</v>
       </c>
       <c r="C28">
         <v>66.180844960000002</v>
@@ -33410,7 +33410,7 @@
         <v>2022</v>
       </c>
       <c r="B29">
-        <v>83</v>
+        <v>97.1</v>
       </c>
       <c r="C29">
         <v>65.587672920000003</v>
@@ -33430,7 +33430,7 @@
         <v>2023</v>
       </c>
       <c r="B30">
-        <v>83</v>
+        <v>97.4</v>
       </c>
       <c r="C30">
         <v>66.98371616</v>
@@ -33450,7 +33450,7 @@
         <v>2024</v>
       </c>
       <c r="B31">
-        <v>83</v>
+        <v>97.6</v>
       </c>
       <c r="C31">
         <v>68.784939679999994</v>
@@ -33470,7 +33470,7 @@
         <v>2025</v>
       </c>
       <c r="B32">
-        <v>83</v>
+        <v>97.8</v>
       </c>
       <c r="C32">
         <v>69.379740209999994</v>
@@ -33490,7 +33490,7 @@
         <v>2026</v>
       </c>
       <c r="B33">
-        <v>83</v>
+        <v>98.1</v>
       </c>
       <c r="C33">
         <v>69.848360650000004</v>
@@ -33510,7 +33510,7 @@
         <v>2027</v>
       </c>
       <c r="B34">
-        <v>83</v>
+        <v>98.3</v>
       </c>
       <c r="C34">
         <v>70.190564620000004</v>
@@ -33530,7 +33530,7 @@
         <v>2028</v>
       </c>
       <c r="B35">
-        <v>83</v>
+        <v>98.5</v>
       </c>
       <c r="C35">
         <v>70.655697110000006</v>
@@ -33550,7 +33550,7 @@
         <v>2029</v>
       </c>
       <c r="B36">
-        <v>83</v>
+        <v>98.8</v>
       </c>
       <c r="C36">
         <v>71.125574380000003</v>
@@ -33570,7 +33570,7 @@
         <v>2030</v>
       </c>
       <c r="B37">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C37">
         <v>71.600236780000003</v>
@@ -33590,7 +33590,7 @@
         <v>2031</v>
       </c>
       <c r="B38">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C38">
         <v>71.600236780000003</v>
@@ -33610,7 +33610,7 @@
         <v>2032</v>
       </c>
       <c r="B39">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C39">
         <v>71.600236780000003</v>
@@ -33630,7 +33630,7 @@
         <v>2033</v>
       </c>
       <c r="B40">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C40">
         <v>71.600236780000003</v>
@@ -33650,7 +33650,7 @@
         <v>2034</v>
       </c>
       <c r="B41">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C41">
         <v>71.600236780000003</v>
@@ -33670,7 +33670,7 @@
         <v>2035</v>
       </c>
       <c r="B42">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C42">
         <v>71.600236780000003</v>
@@ -33690,7 +33690,7 @@
         <v>2036</v>
       </c>
       <c r="B43">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C43">
         <v>71.600236780000003</v>
@@ -33710,7 +33710,7 @@
         <v>2037</v>
       </c>
       <c r="B44">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C44">
         <v>71.600236780000003</v>
@@ -33730,7 +33730,7 @@
         <v>2038</v>
       </c>
       <c r="B45">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C45">
         <v>71.600236780000003</v>
@@ -33750,7 +33750,7 @@
         <v>2039</v>
       </c>
       <c r="B46">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C46">
         <v>71.600236780000003</v>
@@ -33770,7 +33770,7 @@
         <v>2040</v>
       </c>
       <c r="B47">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C47">
         <v>71.600236780000003</v>
@@ -33790,7 +33790,7 @@
         <v>2041</v>
       </c>
       <c r="B48">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C48">
         <v>71.600236780000003</v>
@@ -33810,7 +33810,7 @@
         <v>2042</v>
       </c>
       <c r="B49">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C49">
         <v>71.600236780000003</v>
@@ -33830,7 +33830,7 @@
         <v>2043</v>
       </c>
       <c r="B50">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C50">
         <v>71.600236780000003</v>
@@ -33850,7 +33850,7 @@
         <v>2044</v>
       </c>
       <c r="B51">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C51">
         <v>71.600236780000003</v>
@@ -33870,7 +33870,7 @@
         <v>2045</v>
       </c>
       <c r="B52">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C52">
         <v>71.600236780000003</v>
@@ -33890,7 +33890,7 @@
         <v>2046</v>
       </c>
       <c r="B53">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C53">
         <v>71.600236780000003</v>
@@ -33910,7 +33910,7 @@
         <v>2047</v>
       </c>
       <c r="B54">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C54">
         <v>71.600236780000003</v>
@@ -33930,7 +33930,7 @@
         <v>2048</v>
       </c>
       <c r="B55">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C55">
         <v>71.600236780000003</v>
@@ -33950,7 +33950,7 @@
         <v>2049</v>
       </c>
       <c r="B56">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C56">
         <v>71.600236780000003</v>
@@ -33970,7 +33970,7 @@
         <v>2050</v>
       </c>
       <c r="B57">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C57">
         <v>71.600236780000003</v>

</xml_diff>

<commit_message>
Update for SFs more graphs
Added a module baseline for world with 1TW added annually (all else stayed same). Updated some other things with new data.
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/SupportingMaterial/BaselineGraphs.xlsx
+++ b/PV_ICE/baselines/SupportingMaterial/BaselineGraphs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9F9073-521C-46A4-A955-89DFE0F80845}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5E446E-554B-4769-BD37-34DF2E386981}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2340" windowWidth="29040" windowHeight="15840" xr2:uid="{31D47E9D-A833-4D35-B79A-EFF0E4DE6D01}"/>
+    <workbookView xWindow="28680" yWindow="-2340" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{31D47E9D-A833-4D35-B79A-EFF0E4DE6D01}"/>
   </bookViews>
   <sheets>
     <sheet name="mass per m2" sheetId="1" r:id="rId1"/>
@@ -272,9 +272,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -282,6 +279,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -11878,169 +11878,169 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>99.666666699999993</c:v>
+                  <c:v>99.6666666666666</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>99.333333300000007</c:v>
+                  <c:v>99.3333333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>98.166666700000007</c:v>
+                  <c:v>98.1666666666666</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>97.333333300000007</c:v>
+                  <c:v>97.3333333333333</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>96.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>95.666666700000007</c:v>
+                  <c:v>95.6666666666666</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>94.833333300000007</c:v>
+                  <c:v>94.8333333333333</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>86.082000000000008</c:v>
+                  <c:v>93.768129340000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>78.164000000000001</c:v>
+                  <c:v>93.536258679999989</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>70.245999999999995</c:v>
+                  <c:v>93.30438801999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>62.327999999999996</c:v>
+                  <c:v>93.072517359999992</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>54.410000000000004</c:v>
+                  <c:v>92.840646699999994</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>34.29</c:v>
+                  <c:v>84.828496000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>75.63</c:v>
+                  <c:v>92.755418000000006</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>75.11</c:v>
+                  <c:v>90.832328099999899</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>63.019999999999996</c:v>
+                  <c:v>84.717097199999998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>29.98</c:v>
+                  <c:v>59.613632199999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>81.069999999999993</c:v>
+                  <c:v>91.116584599999996</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>77.02</c:v>
+                  <c:v>85.439676300000002</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>76.92</c:v>
+                  <c:v>89.2007105</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>72.27</c:v>
+                  <c:v>87.078198799999996</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>72.27</c:v>
+                  <c:v>81.800867599999904</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12800,7 +12800,7 @@
                   <a:lumOff val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:prstDash val="sysDash"/>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -39217,7 +39217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56D7BEC5-C527-4A05-96EF-71A772E43E2F}">
   <dimension ref="A1:AI73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
       <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
@@ -39231,21 +39231,21 @@
     <col min="7" max="7" width="11.81640625" customWidth="1"/>
     <col min="8" max="8" width="10.26953125" customWidth="1"/>
     <col min="9" max="9" width="7.6328125" customWidth="1"/>
-    <col min="10" max="10" width="2.453125" style="10" customWidth="1"/>
+    <col min="10" max="10" width="2.453125" style="9" customWidth="1"/>
     <col min="11" max="12" width="8.26953125" customWidth="1"/>
     <col min="13" max="19" width="11.81640625" customWidth="1"/>
-    <col min="20" max="20" width="2.26953125" style="10" customWidth="1"/>
+    <col min="20" max="20" width="2.26953125" style="9" customWidth="1"/>
     <col min="33" max="33" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
       <c r="G1" s="3" t="s">
         <v>38</v>
       </c>
@@ -39253,8 +39253,8 @@
         <v>41</v>
       </c>
       <c r="I1" s="4"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="8" t="s">
+      <c r="J1" s="8"/>
+      <c r="K1" s="7" t="s">
         <v>45</v>
       </c>
       <c r="L1" s="4"/>
@@ -39265,24 +39265,24 @@
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="7" t="s">
+      <c r="T1" s="8"/>
+      <c r="U1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
       <c r="Z1" s="3"/>
       <c r="AA1" s="3"/>
       <c r="AB1" s="3"/>
-      <c r="AC1" s="7" t="s">
+      <c r="AC1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="AD1" s="7"/>
-      <c r="AE1" s="7"/>
-      <c r="AF1" s="7"/>
-      <c r="AG1" s="7"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
       <c r="AH1" s="1" t="s">
         <v>18</v>
       </c>
@@ -39542,7 +39542,7 @@
         <f>AC18*1000/100</f>
         <v>125</v>
       </c>
-      <c r="J18" s="11"/>
+      <c r="J18" s="10"/>
       <c r="K18" s="6">
         <f>H18/I18</f>
         <v>103.96497172550401</v>
@@ -39557,25 +39557,25 @@
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
       <c r="S18" s="6"/>
-      <c r="T18" s="11"/>
+      <c r="T18" s="10"/>
       <c r="U18" s="6">
-        <f>B18/$G18*100</f>
+        <f t="shared" ref="U18:U49" si="1">B18/$G18*100</f>
         <v>66.483930936369333</v>
       </c>
       <c r="V18" s="6">
-        <f>C18/$G18*100</f>
+        <f t="shared" ref="V18:V49" si="2">C18/$G18*100</f>
         <v>7.0507989579972774</v>
       </c>
       <c r="W18" s="6">
-        <f>D18/$G18*100</f>
+        <f t="shared" ref="W18:W49" si="3">D18/$G18*100</f>
         <v>25.689269663744067</v>
       </c>
       <c r="X18" s="6">
-        <f>E18/$G18*100</f>
+        <f t="shared" ref="X18:X49" si="4">E18/$G18*100</f>
         <v>4.4677201589240205E-2</v>
       </c>
       <c r="Y18" s="6">
-        <f>F18/$G18*100</f>
+        <f t="shared" ref="Y18:Y49" si="5">F18/$G18*100</f>
         <v>0.73132324030006279</v>
       </c>
       <c r="AC18">
@@ -39618,16 +39618,16 @@
         <v>11939.14968887</v>
       </c>
       <c r="H19" s="6">
-        <f t="shared" ref="H19:H73" si="1">G19*1.08</f>
+        <f t="shared" ref="H19:H73" si="6">G19*1.08</f>
         <v>12894.281663979602</v>
       </c>
       <c r="I19" s="6">
-        <f t="shared" ref="I19:I73" si="2">AC19*1000/100</f>
+        <f t="shared" ref="I19:I73" si="7">AC19*1000/100</f>
         <v>127</v>
       </c>
-      <c r="J19" s="11"/>
+      <c r="J19" s="10"/>
       <c r="K19" s="6">
-        <f t="shared" ref="K19:K73" si="3">H19/I19</f>
+        <f t="shared" ref="K19:K73" si="8">H19/I19</f>
         <v>101.52977688172915</v>
       </c>
       <c r="L19" s="6">
@@ -39640,25 +39640,25 @@
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
       <c r="S19" s="6"/>
-      <c r="T19" s="11"/>
+      <c r="T19" s="10"/>
       <c r="U19" s="6">
-        <f>B19/$G19*100</f>
+        <f t="shared" si="1"/>
         <v>67.006446928610146</v>
       </c>
       <c r="V19" s="6">
-        <f>C19/$G19*100</f>
+        <f t="shared" si="2"/>
         <v>6.9668756651523793</v>
       </c>
       <c r="W19" s="6">
-        <f>D19/$G19*100</f>
+        <f t="shared" si="3"/>
         <v>25.273295206382389</v>
       </c>
       <c r="X19" s="6">
-        <f>E19/$G19*100</f>
+        <f t="shared" si="4"/>
         <v>4.5028332336026024E-2</v>
       </c>
       <c r="Y19" s="6">
-        <f>F19/$G19*100</f>
+        <f t="shared" si="5"/>
         <v>0.70835386751905605</v>
       </c>
       <c r="AC19">
@@ -39701,16 +39701,16 @@
         <v>11601.668857139999</v>
       </c>
       <c r="H20" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>12529.802365711199</v>
       </c>
       <c r="I20" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>128.80000000000001</v>
       </c>
-      <c r="J20" s="11"/>
+      <c r="J20" s="10"/>
       <c r="K20" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>97.281074267944078</v>
       </c>
       <c r="L20" s="6">
@@ -39723,25 +39723,25 @@
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
       <c r="S20" s="6"/>
-      <c r="T20" s="11"/>
+      <c r="T20" s="10"/>
       <c r="U20" s="6">
-        <f>B20/$G20*100</f>
+        <f t="shared" si="1"/>
         <v>68.955596806890156</v>
       </c>
       <c r="V20" s="6">
-        <f>C20/$G20*100</f>
+        <f t="shared" si="2"/>
         <v>7.0261443421420644</v>
       </c>
       <c r="W20" s="6">
-        <f>D20/$G20*100</f>
+        <f t="shared" si="3"/>
         <v>23.27251392232543</v>
       </c>
       <c r="X20" s="6">
-        <f>E20/$G20*100</f>
+        <f t="shared" si="4"/>
         <v>4.6338161054230192E-2</v>
       </c>
       <c r="Y20" s="6">
-        <f>F20/$G20*100</f>
+        <f t="shared" si="5"/>
         <v>0.69940676758811615</v>
       </c>
       <c r="AC20">
@@ -39784,16 +39784,16 @@
         <v>11421.977242410001</v>
       </c>
       <c r="H21" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>12335.735421802801</v>
       </c>
       <c r="I21" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>130.6</v>
       </c>
-      <c r="J21" s="11"/>
+      <c r="J21" s="10"/>
       <c r="K21" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>94.454329416560498</v>
       </c>
       <c r="L21" s="6">
@@ -39806,25 +39806,25 @@
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
-      <c r="T21" s="11"/>
+      <c r="T21" s="10"/>
       <c r="U21" s="6">
-        <f>B21/$G21*100</f>
+        <f t="shared" si="1"/>
         <v>70.040412708019232</v>
       </c>
       <c r="V21" s="6">
-        <f>C21/$G21*100</f>
+        <f t="shared" si="2"/>
         <v>6.9910337654596475</v>
       </c>
       <c r="W21" s="6">
-        <f>D21/$G21*100</f>
+        <f t="shared" si="3"/>
         <v>22.24109378862665</v>
       </c>
       <c r="X21" s="6">
-        <f>E21/$G21*100</f>
+        <f t="shared" si="4"/>
         <v>4.7067157339788931E-2</v>
       </c>
       <c r="Y21" s="6">
-        <f>F21/$G21*100</f>
+        <f t="shared" si="5"/>
         <v>0.68039258055466523</v>
       </c>
       <c r="AC21">
@@ -39867,16 +39867,16 @@
         <v>11346.239199690001</v>
       </c>
       <c r="H22" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>12253.938335665202</v>
       </c>
       <c r="I22" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>132.4</v>
       </c>
-      <c r="J22" s="11"/>
+      <c r="J22" s="10"/>
       <c r="K22" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>92.55240434792448</v>
       </c>
       <c r="L22" s="6">
@@ -39889,25 +39889,25 @@
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
-      <c r="T22" s="11"/>
+      <c r="T22" s="10"/>
       <c r="U22" s="6">
-        <f>B22/$G22*100</f>
+        <f t="shared" si="1"/>
         <v>70.507944167249477</v>
       </c>
       <c r="V22" s="6">
-        <f>C22/$G22*100</f>
+        <f t="shared" si="2"/>
         <v>6.8910813322299997</v>
       </c>
       <c r="W22" s="6">
-        <f>D22/$G22*100</f>
+        <f t="shared" si="3"/>
         <v>21.89887653759218</v>
       </c>
       <c r="X22" s="6">
-        <f>E22/$G22*100</f>
+        <f t="shared" si="4"/>
         <v>4.7381338480391652E-2</v>
       </c>
       <c r="Y22" s="6">
-        <f>F22/$G22*100</f>
+        <f t="shared" si="5"/>
         <v>0.65471662444794587</v>
       </c>
       <c r="AC22">
@@ -39950,16 +39950,16 @@
         <v>11249.92969253</v>
       </c>
       <c r="H23" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>12149.924067932401</v>
       </c>
       <c r="I23" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>134.19999999999999</v>
       </c>
-      <c r="J23" s="11"/>
+      <c r="J23" s="10"/>
       <c r="K23" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>90.535946854935929</v>
       </c>
       <c r="L23" s="6">
@@ -39974,25 +39974,25 @@
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
       <c r="S23" s="6"/>
-      <c r="T23" s="11"/>
+      <c r="T23" s="10"/>
       <c r="U23" s="6">
-        <f>B23/$G23*100</f>
+        <f t="shared" si="1"/>
         <v>71.111555526538382</v>
       </c>
       <c r="V23" s="6">
-        <f>C23/$G23*100</f>
+        <f t="shared" si="2"/>
         <v>6.8022012404941909</v>
       </c>
       <c r="W23" s="6">
-        <f>D23/$G23*100</f>
+        <f t="shared" si="3"/>
         <v>21.635355335741881</v>
       </c>
       <c r="X23" s="6">
-        <f>E23/$G23*100</f>
+        <f t="shared" si="4"/>
         <v>4.77869653138338E-2</v>
       </c>
       <c r="Y23" s="6">
-        <f>F23/$G23*100</f>
+        <f t="shared" si="5"/>
         <v>0.40310093191170465</v>
       </c>
       <c r="AC23">
@@ -40035,16 +40035,16 @@
         <v>11184.671303610001</v>
       </c>
       <c r="H24" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>12079.445007898801</v>
       </c>
       <c r="I24" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>136</v>
       </c>
-      <c r="J24" s="11"/>
+      <c r="J24" s="10"/>
       <c r="K24" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>88.819448587491181</v>
       </c>
       <c r="L24" s="6">
@@ -40059,25 +40059,25 @@
       </c>
       <c r="R24" s="6"/>
       <c r="S24" s="6"/>
-      <c r="T24" s="11"/>
+      <c r="T24" s="10"/>
       <c r="U24" s="6">
-        <f>B24/$G24*100</f>
+        <f t="shared" si="1"/>
         <v>71.526464952241327</v>
       </c>
       <c r="V24" s="6">
-        <f>C24/$G24*100</f>
+        <f t="shared" si="2"/>
         <v>6.6931528212042952</v>
       </c>
       <c r="W24" s="6">
-        <f>D24/$G24*100</f>
+        <f t="shared" si="3"/>
         <v>21.346482254059556</v>
       </c>
       <c r="X24" s="6">
-        <f>E24/$G24*100</f>
+        <f t="shared" si="4"/>
         <v>4.8065784447906171E-2</v>
       </c>
       <c r="Y24" s="6">
-        <f>F24/$G24*100</f>
+        <f t="shared" si="5"/>
         <v>0.38583418804691544</v>
       </c>
       <c r="AC24">
@@ -40120,16 +40120,16 @@
         <v>11123.194776599999</v>
       </c>
       <c r="H25" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>12013.050358728</v>
       </c>
       <c r="I25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>137.2222222</v>
       </c>
-      <c r="J25" s="11"/>
+      <c r="J25" s="10"/>
       <c r="K25" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>87.544496555514897</v>
       </c>
       <c r="L25" s="6">
@@ -40144,25 +40144,25 @@
       </c>
       <c r="R25" s="6"/>
       <c r="S25" s="6"/>
-      <c r="T25" s="11"/>
+      <c r="T25" s="10"/>
       <c r="U25" s="6">
-        <f>B25/$G25*100</f>
+        <f t="shared" si="1"/>
         <v>71.92178291105445</v>
       </c>
       <c r="V25" s="6">
-        <f>C25/$G25*100</f>
+        <f t="shared" si="2"/>
         <v>6.5805862731079499</v>
       </c>
       <c r="W25" s="6">
-        <f>D25/$G25*100</f>
+        <f t="shared" si="3"/>
         <v>21.081059849216778</v>
       </c>
       <c r="X25" s="6">
-        <f>E25/$G25*100</f>
+        <f t="shared" si="4"/>
         <v>4.8331438116228594E-2</v>
       </c>
       <c r="Y25" s="6">
-        <f>F25/$G25*100</f>
+        <f t="shared" si="5"/>
         <v>0.36823952850459885</v>
       </c>
       <c r="AC25">
@@ -40205,16 +40205,16 @@
         <v>11077.36948159</v>
       </c>
       <c r="H26" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11963.559040117201</v>
       </c>
       <c r="I26" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>138.44444439999998</v>
       </c>
-      <c r="J26" s="11"/>
+      <c r="J26" s="10"/>
       <c r="K26" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>86.414150397769248</v>
       </c>
       <c r="L26" s="6">
@@ -40231,25 +40231,25 @@
         <v>102.7</v>
       </c>
       <c r="S26" s="6"/>
-      <c r="T26" s="11"/>
+      <c r="T26" s="10"/>
       <c r="U26" s="6">
-        <f>B26/$G26*100</f>
+        <f t="shared" si="1"/>
         <v>72.219311753531159</v>
       </c>
       <c r="V26" s="6">
-        <f>C26/$G26*100</f>
+        <f t="shared" si="2"/>
         <v>6.4576316199333235</v>
       </c>
       <c r="W26" s="6">
-        <f>D26/$G26*100</f>
+        <f t="shared" si="3"/>
         <v>20.92457109832992</v>
       </c>
       <c r="X26" s="6">
-        <f>E26/$G26*100</f>
+        <f t="shared" si="4"/>
         <v>4.8531377498372941E-2</v>
       </c>
       <c r="Y26" s="6">
-        <f>F26/$G26*100</f>
+        <f t="shared" si="5"/>
         <v>0.34995415070722846</v>
       </c>
       <c r="AC26">
@@ -40292,16 +40292,16 @@
         <v>10996.66669057</v>
       </c>
       <c r="H27" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11876.400025815601</v>
       </c>
       <c r="I27" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>139.66666670000001</v>
       </c>
-      <c r="J27" s="11"/>
+      <c r="J27" s="10"/>
       <c r="K27" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>85.03389037933988</v>
       </c>
       <c r="L27" s="6">
@@ -40318,25 +40318,25 @@
         <v>102.7</v>
       </c>
       <c r="S27" s="6"/>
-      <c r="T27" s="11"/>
+      <c r="T27" s="10"/>
       <c r="U27" s="6">
-        <f>B27/$G27*100</f>
+        <f t="shared" si="1"/>
         <v>72.749317817009583</v>
       </c>
       <c r="V27" s="6">
-        <f>C27/$G27*100</f>
+        <f t="shared" si="2"/>
         <v>6.3537435448430752</v>
       </c>
       <c r="W27" s="6">
-        <f>D27/$G27*100</f>
+        <f t="shared" si="3"/>
         <v>20.515482786566679</v>
       </c>
       <c r="X27" s="6">
-        <f>E27/$G27*100</f>
+        <f t="shared" si="4"/>
         <v>4.8887541573030449E-2</v>
       </c>
       <c r="Y27" s="6">
-        <f>F27/$G27*100</f>
+        <f t="shared" si="5"/>
         <v>0.33256831000762432</v>
       </c>
       <c r="AC27">
@@ -40379,16 +40379,16 @@
         <v>10735.835995859999</v>
       </c>
       <c r="H28" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11594.702875528799</v>
       </c>
       <c r="I28" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>140.88888890000001</v>
       </c>
-      <c r="J28" s="11"/>
+      <c r="J28" s="10"/>
       <c r="K28" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>82.296786964928629</v>
       </c>
       <c r="L28" s="6">
@@ -40409,25 +40409,25 @@
         <v>102.7</v>
       </c>
       <c r="S28" s="6"/>
-      <c r="T28" s="11"/>
+      <c r="T28" s="10"/>
       <c r="U28" s="6">
-        <f>B28/$G28*100</f>
+        <f t="shared" si="1"/>
         <v>74.516786611540965</v>
       </c>
       <c r="V28" s="6">
-        <f>C28/$G28*100</f>
+        <f t="shared" si="2"/>
         <v>5.4234248755712162</v>
       </c>
       <c r="W28" s="6">
-        <f>D28/$G28*100</f>
+        <f t="shared" si="3"/>
         <v>19.68950395493323</v>
       </c>
       <c r="X28" s="6">
-        <f>E28/$G28*100</f>
+        <f t="shared" si="4"/>
         <v>5.0075280602955533E-2</v>
       </c>
       <c r="Y28" s="6">
-        <f>F28/$G28*100</f>
+        <f t="shared" si="5"/>
         <v>0.3202092773516349</v>
       </c>
       <c r="AC28">
@@ -40470,16 +40470,16 @@
         <v>10586.83833814</v>
       </c>
       <c r="H29" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11433.7854051912</v>
       </c>
       <c r="I29" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>142.11111109999999</v>
       </c>
-      <c r="J29" s="11"/>
+      <c r="J29" s="10"/>
       <c r="K29" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>80.456660402475748</v>
       </c>
       <c r="L29" s="6">
@@ -40498,25 +40498,25 @@
         <v>102.7</v>
       </c>
       <c r="S29" s="6"/>
-      <c r="T29" s="11"/>
+      <c r="T29" s="10"/>
       <c r="U29" s="6">
-        <f>B29/$G29*100</f>
+        <f t="shared" si="1"/>
         <v>75.565525272822086</v>
       </c>
       <c r="V29" s="6">
-        <f>C29/$G29*100</f>
+        <f t="shared" si="2"/>
         <v>4.3998027090100669</v>
       </c>
       <c r="W29" s="6">
-        <f>D29/$G29*100</f>
+        <f t="shared" si="3"/>
         <v>19.679902672113968</v>
       </c>
       <c r="X29" s="6">
-        <f>E29/$G29*100</f>
+        <f t="shared" si="4"/>
         <v>5.078003298333645E-2</v>
       </c>
       <c r="Y29" s="6">
-        <f>F29/$G29*100</f>
+        <f t="shared" si="5"/>
         <v>0.30398931307053662</v>
       </c>
       <c r="AC29">
@@ -40559,16 +40559,16 @@
         <v>10532.556731430001</v>
       </c>
       <c r="H30" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11375.161269944401</v>
       </c>
       <c r="I30" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>143.33333329999999</v>
       </c>
-      <c r="J30" s="11"/>
+      <c r="J30" s="10"/>
       <c r="K30" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>79.361590273882243</v>
       </c>
       <c r="L30" s="6">
@@ -40589,25 +40589,25 @@
         <v>102.7</v>
       </c>
       <c r="S30" s="6"/>
-      <c r="T30" s="11"/>
+      <c r="T30" s="10"/>
       <c r="U30" s="6">
-        <f>B30/$G30*100</f>
+        <f t="shared" si="1"/>
         <v>75.954967098609146</v>
       </c>
       <c r="V30" s="6">
-        <f>C30/$G30*100</f>
+        <f t="shared" si="2"/>
         <v>4.201354061350691</v>
       </c>
       <c r="W30" s="6">
-        <f>D30/$G30*100</f>
+        <f t="shared" si="3"/>
         <v>19.507914482612396</v>
       </c>
       <c r="X30" s="6">
-        <f>E30/$G30*100</f>
+        <f t="shared" si="4"/>
         <v>5.1041737890265351E-2</v>
       </c>
       <c r="Y30" s="6">
-        <f>F30/$G30*100</f>
+        <f t="shared" si="5"/>
         <v>0.28472261953749256</v>
       </c>
       <c r="AC30">
@@ -40650,16 +40650,16 @@
         <v>10479.71451071</v>
       </c>
       <c r="H31" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11318.091671566801</v>
       </c>
       <c r="I31" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>144.55555560000002</v>
       </c>
-      <c r="J31" s="11"/>
+      <c r="J31" s="10"/>
       <c r="K31" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>78.295791708518735</v>
       </c>
       <c r="L31" s="6">
@@ -40680,25 +40680,25 @@
         <v>102.7</v>
       </c>
       <c r="S31" s="6"/>
-      <c r="T31" s="11"/>
+      <c r="T31" s="10"/>
       <c r="U31" s="6">
-        <f>B31/$G31*100</f>
+        <f t="shared" si="1"/>
         <v>76.337957411189066</v>
       </c>
       <c r="V31" s="6">
-        <f>C31/$G31*100</f>
+        <f t="shared" si="2"/>
         <v>4.0002998132398346</v>
       </c>
       <c r="W31" s="6">
-        <f>D31/$G31*100</f>
+        <f t="shared" si="3"/>
         <v>19.345223793340232</v>
       </c>
       <c r="X31" s="6">
-        <f>E31/$G31*100</f>
+        <f t="shared" si="4"/>
         <v>5.1299107380319051E-2</v>
       </c>
       <c r="Y31" s="6">
-        <f>F31/$G31*100</f>
+        <f t="shared" si="5"/>
         <v>0.2652198748505501</v>
       </c>
       <c r="AC31">
@@ -40741,16 +40741,16 @@
         <v>10451.49639</v>
       </c>
       <c r="H32" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11287.616101200001</v>
       </c>
       <c r="I32" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>145.7777778</v>
       </c>
-      <c r="J32" s="11"/>
+      <c r="J32" s="10"/>
       <c r="K32" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>77.430293365330755</v>
       </c>
       <c r="L32" s="6">
@@ -40771,25 +40771,25 @@
         <v>102.7</v>
       </c>
       <c r="S32" s="6"/>
-      <c r="T32" s="11"/>
+      <c r="T32" s="10"/>
       <c r="U32" s="6">
-        <f>B32/$G32*100</f>
+        <f t="shared" si="1"/>
         <v>76.544063179837167</v>
       </c>
       <c r="V32" s="6">
-        <f>C32/$G32*100</f>
+        <f t="shared" si="2"/>
         <v>4.0111002707814167</v>
       </c>
       <c r="W32" s="6">
-        <f>D32/$G32*100</f>
+        <f t="shared" si="3"/>
         <v>19.148457936749093</v>
       </c>
       <c r="X32" s="6">
-        <f>E32/$G32*100</f>
+        <f t="shared" si="4"/>
         <v>5.1437610456850573E-2</v>
       </c>
       <c r="Y32" s="6">
-        <f>F32/$G32*100</f>
+        <f t="shared" si="5"/>
         <v>0.24494100217547893</v>
       </c>
       <c r="AC32">
@@ -40831,20 +40831,20 @@
         <v>12.327416169999999</v>
       </c>
       <c r="G33" s="6">
-        <f t="shared" ref="G33:G73" si="4">SUM(B33:F33)</f>
+        <f t="shared" ref="G33:G73" si="9">SUM(B33:F33)</f>
         <v>10424.07407517</v>
       </c>
       <c r="H33" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11258.0000011836</v>
       </c>
       <c r="I33" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>147</v>
       </c>
-      <c r="J33" s="11"/>
+      <c r="J33" s="10"/>
       <c r="K33" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>76.585034021657137</v>
       </c>
       <c r="L33" s="6">
@@ -40867,25 +40867,25 @@
         <v>102.7</v>
       </c>
       <c r="S33" s="6"/>
-      <c r="T33" s="11"/>
+      <c r="T33" s="10"/>
       <c r="U33" s="6">
-        <f>B33/$G33*100</f>
+        <f t="shared" si="1"/>
         <v>76.745425467149062</v>
       </c>
       <c r="V33" s="6">
-        <f>C33/$G33*100</f>
+        <f t="shared" si="2"/>
         <v>4.0216521580422793</v>
       </c>
       <c r="W33" s="6">
-        <f>D33/$G33*100</f>
+        <f t="shared" si="3"/>
         <v>19.063090349035079</v>
       </c>
       <c r="X33" s="6">
-        <f>E33/$G33*100</f>
+        <f t="shared" si="4"/>
         <v>5.1572925913924178E-2</v>
       </c>
       <c r="Y33" s="6">
-        <f>F33/$G33*100</f>
+        <f t="shared" si="5"/>
         <v>0.11825909985965789</v>
       </c>
       <c r="AC33">
@@ -40930,20 +40930,20 @@
         <v>10.272846810000001</v>
       </c>
       <c r="G34" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10401.461976809998</v>
       </c>
       <c r="H34" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11233.578934954799</v>
       </c>
       <c r="I34" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>151</v>
       </c>
-      <c r="J34" s="11"/>
+      <c r="J34" s="10"/>
       <c r="K34" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>74.394562483144369</v>
       </c>
       <c r="L34" s="6">
@@ -40964,25 +40964,25 @@
         <v>102.7</v>
       </c>
       <c r="S34" s="6"/>
-      <c r="T34" s="11"/>
+      <c r="T34" s="10"/>
       <c r="U34" s="6">
-        <f>B34/$G34*100</f>
+        <f t="shared" si="1"/>
         <v>76.912265005015215</v>
       </c>
       <c r="V34" s="6">
-        <f>C34/$G34*100</f>
+        <f t="shared" si="2"/>
         <v>4.0303949669253107</v>
       </c>
       <c r="W34" s="6">
-        <f>D34/$G34*100</f>
+        <f t="shared" si="3"/>
         <v>18.906891496450292</v>
       </c>
       <c r="X34" s="6">
-        <f>E34/$G34*100</f>
+        <f t="shared" si="4"/>
         <v>5.1685042083370235E-2</v>
       </c>
       <c r="Y34" s="6">
-        <f>F34/$G34*100</f>
+        <f t="shared" si="5"/>
         <v>9.8763489525830653E-2</v>
       </c>
       <c r="AC34">
@@ -41024,20 +41024,20 @@
         <v>8.2182774490000003</v>
       </c>
       <c r="G35" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10475.800475448999</v>
       </c>
       <c r="H35" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11313.864513484919</v>
       </c>
       <c r="I35" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>154</v>
       </c>
-      <c r="J35" s="11"/>
+      <c r="J35" s="10"/>
       <c r="K35" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>73.466652684967002</v>
       </c>
       <c r="L35" s="6">
@@ -41062,25 +41062,25 @@
         <v>102.7</v>
       </c>
       <c r="S35" s="6"/>
-      <c r="T35" s="11"/>
+      <c r="T35" s="10"/>
       <c r="U35" s="6">
-        <f>B35/$G35*100</f>
+        <f t="shared" si="1"/>
         <v>77.130144077640864</v>
       </c>
       <c r="V35" s="6">
-        <f>C35/$G35*100</f>
+        <f t="shared" si="2"/>
         <v>4.001794430721362</v>
       </c>
       <c r="W35" s="6">
-        <f>D35/$G35*100</f>
+        <f t="shared" si="3"/>
         <v>18.73829310323768</v>
       </c>
       <c r="X35" s="6">
-        <f>E35/$G35*100</f>
+        <f t="shared" si="4"/>
         <v>5.131827407938086E-2</v>
       </c>
       <c r="Y35" s="6">
-        <f>F35/$G35*100</f>
+        <f t="shared" si="5"/>
         <v>7.845011432071744E-2</v>
       </c>
       <c r="AC35">
@@ -41122,20 +41122,20 @@
         <v>5.7527942139999997</v>
       </c>
       <c r="G36" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10209.806922214</v>
       </c>
       <c r="H36" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11026.591475991121</v>
       </c>
       <c r="I36" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>160</v>
       </c>
-      <c r="J36" s="11"/>
+      <c r="J36" s="10"/>
       <c r="K36" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>68.916196724944513</v>
       </c>
       <c r="L36" s="6">
@@ -41158,25 +41158,25 @@
         <v>102.7</v>
       </c>
       <c r="S36" s="6"/>
-      <c r="T36" s="11"/>
+      <c r="T36" s="10"/>
       <c r="U36" s="6">
-        <f>B36/$G36*100</f>
+        <f t="shared" si="1"/>
         <v>79.923156844874995</v>
       </c>
       <c r="V36" s="6">
-        <f>C36/$G36*100</f>
+        <f t="shared" si="2"/>
         <v>4.1060521829054526</v>
       </c>
       <c r="W36" s="6">
-        <f>D36/$G36*100</f>
+        <f t="shared" si="3"/>
         <v>15.861789947040645</v>
       </c>
       <c r="X36" s="6">
-        <f>E36/$G36*100</f>
+        <f t="shared" si="4"/>
         <v>5.2655256274270583E-2</v>
       </c>
       <c r="Y36" s="6">
-        <f>F36/$G36*100</f>
+        <f t="shared" si="5"/>
         <v>5.634576890463374E-2</v>
       </c>
       <c r="AC36">
@@ -41218,20 +41218,20 @@
         <v>5.3418803419999996</v>
       </c>
       <c r="G37" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10315.377606342001</v>
       </c>
       <c r="H37" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11140.607814849362</v>
       </c>
       <c r="I37" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>163</v>
       </c>
-      <c r="J37" s="11"/>
+      <c r="J37" s="10"/>
       <c r="K37" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>68.347287207664792</v>
       </c>
       <c r="L37" s="6">
@@ -41254,25 +41254,25 @@
         <v>102.7</v>
       </c>
       <c r="S37" s="6"/>
-      <c r="T37" s="11"/>
+      <c r="T37" s="10"/>
       <c r="U37" s="6">
-        <f>B37/$G37*100</f>
+        <f t="shared" si="1"/>
         <v>80.391628076722682</v>
       </c>
       <c r="V37" s="6">
-        <f>C37/$G37*100</f>
+        <f t="shared" si="2"/>
         <v>4.0640296070427828</v>
       </c>
       <c r="W37" s="6">
-        <f>D37/$G37*100</f>
+        <f t="shared" si="3"/>
         <v>15.440440348211462</v>
       </c>
       <c r="X37" s="6">
-        <f>E37/$G37*100</f>
+        <f t="shared" si="4"/>
         <v>5.2116366507948091E-2</v>
       </c>
       <c r="Y37" s="6">
-        <f>F37/$G37*100</f>
+        <f t="shared" si="5"/>
         <v>5.1785601515118136E-2</v>
       </c>
       <c r="AC37">
@@ -41314,20 +41314,20 @@
         <v>4.5200525970000003</v>
       </c>
       <c r="G38" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10150.433136596999</v>
       </c>
       <c r="H38" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>10962.46778752476</v>
       </c>
       <c r="I38" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>170</v>
       </c>
-      <c r="J38" s="11"/>
+      <c r="J38" s="10"/>
       <c r="K38" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>64.48510463249859</v>
       </c>
       <c r="L38" s="6">
@@ -41352,25 +41352,25 @@
         <v>102.7</v>
       </c>
       <c r="S38" s="6"/>
-      <c r="T38" s="11"/>
+      <c r="T38" s="10"/>
       <c r="U38" s="6">
-        <f>B38/$G38*100</f>
+        <f t="shared" si="1"/>
         <v>81.037551691687796</v>
       </c>
       <c r="V38" s="6">
-        <f>C38/$G38*100</f>
+        <f t="shared" si="2"/>
         <v>4.1300700606412377</v>
       </c>
       <c r="W38" s="6">
-        <f>D38/$G38*100</f>
+        <f t="shared" si="3"/>
         <v>14.73082383656083</v>
       </c>
       <c r="X38" s="6">
-        <f>E38/$G38*100</f>
+        <f t="shared" si="4"/>
         <v>5.7023773489340179E-2</v>
       </c>
       <c r="Y38" s="6">
-        <f>F38/$G38*100</f>
+        <f t="shared" si="5"/>
         <v>4.4530637620803816E-2</v>
       </c>
       <c r="AC38">
@@ -41415,20 +41415,20 @@
         <v>4.0997570090000002</v>
       </c>
       <c r="G39" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10000.933893009</v>
       </c>
       <c r="H39" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>10801.00860444972</v>
       </c>
       <c r="I39" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>175</v>
       </c>
-      <c r="J39" s="11"/>
+      <c r="J39" s="10"/>
       <c r="K39" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>61.720049168284113</v>
       </c>
       <c r="L39" s="6">
@@ -41451,25 +41451,25 @@
         <v>102.7</v>
       </c>
       <c r="S39" s="6"/>
-      <c r="T39" s="11"/>
+      <c r="T39" s="10"/>
       <c r="U39" s="6">
-        <f>B39/$G39*100</f>
+        <f t="shared" si="1"/>
         <v>81.581256183518477</v>
       </c>
       <c r="V39" s="6">
-        <f>C39/$G39*100</f>
+        <f t="shared" si="2"/>
         <v>4.1918085299318832</v>
       </c>
       <c r="W39" s="6">
-        <f>D39/$G39*100</f>
+        <f t="shared" si="3"/>
         <v>14.123944134731307</v>
       </c>
       <c r="X39" s="6">
-        <f>E39/$G39*100</f>
+        <f t="shared" si="4"/>
         <v>6.1997410105212668E-2</v>
       </c>
       <c r="Y39" s="6">
-        <f>F39/$G39*100</f>
+        <f t="shared" si="5"/>
         <v>4.099374171312014E-2</v>
       </c>
       <c r="AC39">
@@ -41511,20 +41511,20 @@
         <v>4.079110301</v>
       </c>
       <c r="G40" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10100.073846300998</v>
       </c>
       <c r="H40" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>10908.079754005079</v>
       </c>
       <c r="I40" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>177</v>
       </c>
-      <c r="J40" s="11"/>
+      <c r="J40" s="10"/>
       <c r="K40" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>61.62756923166711</v>
       </c>
       <c r="L40" s="6">
@@ -41547,25 +41547,25 @@
         <v>102.7</v>
       </c>
       <c r="S40" s="6"/>
-      <c r="T40" s="11"/>
+      <c r="T40" s="10"/>
       <c r="U40" s="6">
-        <f>B40/$G40*100</f>
+        <f t="shared" si="1"/>
         <v>82.076132572396958</v>
       </c>
       <c r="V40" s="6">
-        <f>C40/$G40*100</f>
+        <f t="shared" si="2"/>
         <v>4.1506627216743874</v>
       </c>
       <c r="W40" s="6">
-        <f>D40/$G40*100</f>
+        <f t="shared" si="3"/>
         <v>13.661493143491606</v>
       </c>
       <c r="X40" s="6">
-        <f>E40/$G40*100</f>
+        <f t="shared" si="4"/>
         <v>7.1324627023774678E-2</v>
       </c>
       <c r="Y40" s="6">
-        <f>F40/$G40*100</f>
+        <f t="shared" si="5"/>
         <v>4.0386935413288229E-2</v>
       </c>
       <c r="AC40">
@@ -41607,20 +41607,20 @@
         <v>4.3128338230000001</v>
       </c>
       <c r="G41" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10134.439229122998</v>
       </c>
       <c r="H41" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>10945.194367452839</v>
       </c>
       <c r="I41" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>184</v>
       </c>
-      <c r="J41" s="11"/>
+      <c r="J41" s="10"/>
       <c r="K41" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>59.484751997026301</v>
       </c>
       <c r="L41" s="6">
@@ -41643,25 +41643,25 @@
         <v>102.7</v>
       </c>
       <c r="S41" s="6"/>
-      <c r="T41" s="11"/>
+      <c r="T41" s="10"/>
       <c r="U41" s="6">
-        <f>B41/$G41*100</f>
+        <f t="shared" si="1"/>
         <v>82.393804049901973</v>
       </c>
       <c r="V41" s="6">
-        <f>C41/$G41*100</f>
+        <f t="shared" si="2"/>
         <v>4.0540477772005357</v>
       </c>
       <c r="W41" s="6">
-        <f>D41/$G41*100</f>
+        <f t="shared" si="3"/>
         <v>13.436033669105482</v>
       </c>
       <c r="X41" s="6">
-        <f>E41/$G41*100</f>
+        <f t="shared" si="4"/>
         <v>7.3558288045949521E-2</v>
       </c>
       <c r="Y41" s="6">
-        <f>F41/$G41*100</f>
+        <f t="shared" si="5"/>
         <v>4.255621574607063E-2</v>
       </c>
       <c r="AC41">
@@ -41703,20 +41703,20 @@
         <v>4.1473098100000003</v>
       </c>
       <c r="G42" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10365.696155509999</v>
       </c>
       <c r="H42" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11194.951847950799</v>
       </c>
       <c r="I42" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>192</v>
       </c>
-      <c r="J42" s="11"/>
+      <c r="J42" s="10"/>
       <c r="K42" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>58.307040874743741</v>
       </c>
       <c r="L42" s="6">
@@ -41739,25 +41739,25 @@
         <v>102.7</v>
       </c>
       <c r="S42" s="6"/>
-      <c r="T42" s="11"/>
+      <c r="T42" s="10"/>
       <c r="U42" s="6">
-        <f>B42/$G42*100</f>
+        <f t="shared" si="1"/>
         <v>83.038320541786177</v>
       </c>
       <c r="V42" s="6">
-        <f>C42/$G42*100</f>
+        <f t="shared" si="2"/>
         <v>3.8795336142111183</v>
       </c>
       <c r="W42" s="6">
-        <f>D42/$G42*100</f>
+        <f t="shared" si="3"/>
         <v>12.962439172845809</v>
       </c>
       <c r="X42" s="6">
-        <f>E42/$G42*100</f>
+        <f t="shared" si="4"/>
         <v>7.9696721532867928E-2</v>
       </c>
       <c r="Y42" s="6">
-        <f>F42/$G42*100</f>
+        <f t="shared" si="5"/>
         <v>4.0009949624034202E-2</v>
       </c>
       <c r="AC42">
@@ -41799,20 +41799,20 @@
         <v>3.5949654450000001</v>
       </c>
       <c r="G43" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10605.058052745</v>
       </c>
       <c r="H43" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11453.462696964601</v>
       </c>
       <c r="I43" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>202.52588490000002</v>
       </c>
-      <c r="J43" s="11"/>
+      <c r="J43" s="10"/>
       <c r="K43" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>56.553080622854253</v>
       </c>
       <c r="L43" s="6">
@@ -41839,25 +41839,25 @@
       <c r="S43" s="6">
         <v>76</v>
       </c>
-      <c r="T43" s="11"/>
+      <c r="T43" s="10"/>
       <c r="U43" s="6">
-        <f>B43/$G43*100</f>
+        <f t="shared" si="1"/>
         <v>83.90453834146453</v>
       </c>
       <c r="V43" s="6">
-        <f>C43/$G43*100</f>
+        <f t="shared" si="2"/>
         <v>3.5837048831772056</v>
       </c>
       <c r="W43" s="6">
-        <f>D43/$G43*100</f>
+        <f t="shared" si="3"/>
         <v>12.400298211093826</v>
       </c>
       <c r="X43" s="6">
-        <f>E43/$G43*100</f>
+        <f t="shared" si="4"/>
         <v>7.7559971469189443E-2</v>
       </c>
       <c r="Y43" s="6">
-        <f>F43/$G43*100</f>
+        <f t="shared" si="5"/>
         <v>3.3898592795250981E-2</v>
       </c>
       <c r="AC43">
@@ -41902,20 +41902,20 @@
         <v>3.3412788689999999</v>
       </c>
       <c r="G44" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10597.359347469001</v>
       </c>
       <c r="H44" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11445.148095266521</v>
       </c>
       <c r="I44" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>208.94864799999999</v>
       </c>
-      <c r="J44" s="11"/>
+      <c r="J44" s="10"/>
       <c r="K44" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>54.774932524409159</v>
       </c>
       <c r="L44" s="6">
@@ -41940,25 +41940,25 @@
       <c r="S44" s="6">
         <v>76</v>
       </c>
-      <c r="T44" s="11"/>
+      <c r="T44" s="10"/>
       <c r="U44" s="6">
-        <f>B44/$G44*100</f>
+        <f t="shared" si="1"/>
         <v>84.21673463523274</v>
       </c>
       <c r="V44" s="6">
-        <f>C44/$G44*100</f>
+        <f t="shared" si="2"/>
         <v>3.4667159011432651</v>
       </c>
       <c r="W44" s="6">
-        <f>D44/$G44*100</f>
+        <f t="shared" si="3"/>
         <v>12.206981046735558</v>
       </c>
       <c r="X44" s="6">
-        <f>E44/$G44*100</f>
+        <f t="shared" si="4"/>
         <v>7.80390635896967E-2</v>
       </c>
       <c r="Y44" s="6">
-        <f>F44/$G44*100</f>
+        <f t="shared" si="5"/>
         <v>3.1529353298734818E-2</v>
       </c>
       <c r="AC44">
@@ -42000,20 +42000,20 @@
         <v>3.0936340219999998</v>
       </c>
       <c r="G45" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10588.791685022001</v>
       </c>
       <c r="H45" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11435.895019823762</v>
       </c>
       <c r="I45" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>213.6288232</v>
       </c>
-      <c r="J45" s="11"/>
+      <c r="J45" s="10"/>
       <c r="K45" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>53.531610802899195</v>
       </c>
       <c r="L45" s="6">
@@ -42038,25 +42038,25 @@
       <c r="S45" s="6">
         <v>76</v>
       </c>
-      <c r="T45" s="11"/>
+      <c r="T45" s="10"/>
       <c r="U45" s="6">
-        <f>B45/$G45*100</f>
+        <f t="shared" si="1"/>
         <v>84.528058217073166</v>
       </c>
       <c r="V45" s="6">
-        <f>C45/$G45*100</f>
+        <f t="shared" si="2"/>
         <v>3.3498316951662934</v>
       </c>
       <c r="W45" s="6">
-        <f>D45/$G45*100</f>
+        <f t="shared" si="3"/>
         <v>12.01436867248519</v>
       </c>
       <c r="X45" s="6">
-        <f>E45/$G45*100</f>
+        <f t="shared" si="4"/>
         <v>7.8525295872630296E-2</v>
       </c>
       <c r="Y45" s="6">
-        <f>F45/$G45*100</f>
+        <f t="shared" si="5"/>
         <v>2.9216119402707581E-2</v>
       </c>
       <c r="AC45">
@@ -42098,20 +42098,20 @@
         <v>2.8988638820000001</v>
       </c>
       <c r="G46" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10529.900575282001</v>
       </c>
       <c r="H46" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11372.292621304561</v>
       </c>
       <c r="I46" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>217.3311205</v>
       </c>
-      <c r="J46" s="11"/>
+      <c r="J46" s="10"/>
       <c r="K46" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>52.327032571962292</v>
       </c>
       <c r="L46" s="6">
@@ -42136,25 +42136,25 @@
       <c r="S46" s="6">
         <v>76</v>
       </c>
-      <c r="T46" s="11"/>
+      <c r="T46" s="10"/>
       <c r="U46" s="6">
-        <f>B46/$G46*100</f>
+        <f t="shared" si="1"/>
         <v>84.908921371848351</v>
       </c>
       <c r="V46" s="6">
-        <f>C46/$G46*100</f>
+        <f t="shared" si="2"/>
         <v>3.3095852226569278</v>
       </c>
       <c r="W46" s="6">
-        <f>D46/$G46*100</f>
+        <f t="shared" si="3"/>
         <v>11.674318377570039</v>
       </c>
       <c r="X46" s="6">
-        <f>E46/$G46*100</f>
+        <f t="shared" si="4"/>
         <v>7.9645196457853534E-2</v>
       </c>
       <c r="Y46" s="6">
-        <f>F46/$G46*100</f>
+        <f t="shared" si="5"/>
         <v>2.7529831466830974E-2</v>
       </c>
       <c r="AC46">
@@ -42196,20 +42196,20 @@
         <v>2.692895407</v>
       </c>
       <c r="G47" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10467.848267107001</v>
       </c>
       <c r="H47" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11305.276128475562</v>
       </c>
       <c r="I47" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>220.40369699999999</v>
       </c>
-      <c r="J47" s="11"/>
+      <c r="J47" s="10"/>
       <c r="K47" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>51.293495900277762</v>
       </c>
       <c r="L47" s="6">
@@ -42234,25 +42234,25 @@
       <c r="S47" s="6">
         <v>76</v>
       </c>
-      <c r="T47" s="11"/>
+      <c r="T47" s="10"/>
       <c r="U47" s="6">
-        <f>B47/$G47*100</f>
+        <f t="shared" si="1"/>
         <v>85.289734548926845</v>
       </c>
       <c r="V47" s="6">
-        <f>C47/$G47*100</f>
+        <f t="shared" si="2"/>
         <v>3.269873215258186</v>
       </c>
       <c r="W47" s="6">
-        <f>D47/$G47*100</f>
+        <f t="shared" si="3"/>
         <v>11.333864751632367</v>
       </c>
       <c r="X47" s="6">
-        <f>E47/$G47*100</f>
+        <f t="shared" si="4"/>
         <v>8.0802088300976141E-2</v>
       </c>
       <c r="Y47" s="6">
-        <f>F47/$G47*100</f>
+        <f t="shared" si="5"/>
         <v>2.5725395881614505E-2</v>
       </c>
       <c r="AC47">
@@ -42294,20 +42294,20 @@
         <v>2.542951049</v>
       </c>
       <c r="G48" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10450.506525882</v>
       </c>
       <c r="H48" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11286.547047952561</v>
       </c>
       <c r="I48" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>223.03538889999999</v>
       </c>
-      <c r="J48" s="11"/>
+      <c r="J48" s="10"/>
       <c r="K48" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>50.604287972492969</v>
       </c>
       <c r="L48" s="6">
@@ -42334,25 +42334,25 @@
       <c r="S48" s="6">
         <v>76</v>
       </c>
-      <c r="T48" s="11"/>
+      <c r="T48" s="10"/>
       <c r="U48" s="6">
-        <f>B48/$G48*100</f>
+        <f t="shared" si="1"/>
         <v>85.602868251833215</v>
       </c>
       <c r="V48" s="6">
-        <f>C48/$G48*100</f>
+        <f t="shared" si="2"/>
         <v>3.2152632857347685</v>
       </c>
       <c r="W48" s="6">
-        <f>D48/$G48*100</f>
+        <f t="shared" si="3"/>
         <v>11.079113975313099</v>
       </c>
       <c r="X48" s="6">
-        <f>E48/$G48*100</f>
+        <f t="shared" si="4"/>
         <v>7.8421206787470277E-2</v>
       </c>
       <c r="Y48" s="6">
-        <f>F48/$G48*100</f>
+        <f t="shared" si="5"/>
         <v>2.4333280331456285E-2</v>
       </c>
       <c r="AC48">
@@ -42397,20 +42397,20 @@
         <v>2.4012622069999998</v>
       </c>
       <c r="G49" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10432.239708074001</v>
       </c>
       <c r="H49" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11266.818884719922</v>
       </c>
       <c r="I49" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>225.34045020000002</v>
       </c>
-      <c r="J49" s="11"/>
+      <c r="J49" s="10"/>
       <c r="K49" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>49.999096366054566</v>
       </c>
       <c r="L49" s="6">
@@ -42435,25 +42435,25 @@
       <c r="S49" s="6">
         <v>76</v>
       </c>
-      <c r="T49" s="11"/>
+      <c r="T49" s="10"/>
       <c r="U49" s="6">
-        <f>B49/$G49*100</f>
+        <f t="shared" si="1"/>
         <v>85.915714974064144</v>
       </c>
       <c r="V49" s="6">
-        <f>C49/$G49*100</f>
+        <f t="shared" si="2"/>
         <v>3.160752066929605</v>
       </c>
       <c r="W49" s="6">
-        <f>D49/$G49*100</f>
+        <f t="shared" si="3"/>
         <v>10.824476101004771</v>
       </c>
       <c r="X49" s="6">
-        <f>E49/$G49*100</f>
+        <f t="shared" si="4"/>
         <v>7.6039152559546713E-2</v>
       </c>
       <c r="Y49" s="6">
-        <f>F49/$G49*100</f>
+        <f t="shared" si="5"/>
         <v>2.3017705441924899E-2</v>
       </c>
       <c r="AC49">
@@ -42495,20 +42495,20 @@
         <v>2.2668844890000002</v>
       </c>
       <c r="G50" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10413.046868489</v>
       </c>
       <c r="H50" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11246.090617968121</v>
       </c>
       <c r="I50" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>227.39342440000001</v>
       </c>
-      <c r="J50" s="11"/>
+      <c r="J50" s="10"/>
       <c r="K50" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>49.456533968130522</v>
       </c>
       <c r="L50" s="6">
@@ -42533,25 +42533,25 @@
       <c r="S50" s="6">
         <v>76</v>
       </c>
-      <c r="T50" s="11"/>
+      <c r="T50" s="10"/>
       <c r="U50" s="6">
-        <f>B50/$G50*100</f>
+        <f t="shared" ref="U50:U73" si="10">B50/$G50*100</f>
         <v>86.228364410530219</v>
       </c>
       <c r="V50" s="6">
-        <f>C50/$G50*100</f>
+        <f t="shared" ref="V50:V73" si="11">C50/$G50*100</f>
         <v>3.1063258341690014</v>
       </c>
       <c r="W50" s="6">
-        <f>D50/$G50*100</f>
+        <f t="shared" ref="W50:W73" si="12">D50/$G50*100</f>
         <v>10.569884807977541</v>
       </c>
       <c r="X50" s="6">
-        <f>E50/$G50*100</f>
+        <f t="shared" ref="X50:X73" si="13">E50/$G50*100</f>
         <v>7.3655291259751454E-2</v>
       </c>
       <c r="Y50" s="6">
-        <f>F50/$G50*100</f>
+        <f t="shared" ref="Y50:Y73" si="14">F50/$G50*100</f>
         <v>2.176965606348932E-2</v>
       </c>
       <c r="AC50">
@@ -42593,20 +42593,20 @@
         <v>2.1296348279999999</v>
       </c>
       <c r="G51" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10451.590593794999</v>
       </c>
       <c r="H51" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11287.7178412986</v>
       </c>
       <c r="I51" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>229.24571610000004</v>
       </c>
-      <c r="J51" s="11"/>
+      <c r="J51" s="10"/>
       <c r="K51" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>49.238511555761185</v>
       </c>
       <c r="L51" s="6">
@@ -42631,25 +42631,25 @@
       <c r="S51" s="6">
         <v>76</v>
       </c>
-      <c r="T51" s="11"/>
+      <c r="T51" s="10"/>
       <c r="U51" s="6">
-        <f>B51/$G51*100</f>
+        <f t="shared" si="10"/>
         <v>86.494676220545756</v>
       </c>
       <c r="V51" s="6">
-        <f>C51/$G51*100</f>
+        <f t="shared" si="11"/>
         <v>3.0656414487783619</v>
       </c>
       <c r="W51" s="6">
-        <f>D51/$G51*100</f>
+        <f t="shared" si="12"/>
         <v>10.34855149839229</v>
       </c>
       <c r="X51" s="6">
-        <f>E51/$G51*100</f>
+        <f t="shared" si="13"/>
         <v>7.0754653089744324E-2</v>
       </c>
       <c r="Y51" s="6">
-        <f>F51/$G51*100</f>
+        <f t="shared" si="14"/>
         <v>2.0376179193857268E-2</v>
       </c>
       <c r="AC51">
@@ -42691,20 +42691,20 @@
         <v>1.9927764130000001</v>
       </c>
       <c r="G52" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10489.356934446001</v>
       </c>
       <c r="H52" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11328.505489201681</v>
       </c>
       <c r="I52" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>230.93431240000001</v>
       </c>
-      <c r="J52" s="11"/>
+      <c r="J52" s="10"/>
       <c r="K52" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>49.055098705209474</v>
       </c>
       <c r="L52" s="6">
@@ -42729,25 +42729,25 @@
       <c r="S52" s="6">
         <v>76</v>
       </c>
-      <c r="T52" s="11"/>
+      <c r="T52" s="10"/>
       <c r="U52" s="6">
-        <f>B52/$G52*100</f>
+        <f t="shared" si="10"/>
         <v>86.75804596862676</v>
       </c>
       <c r="V52" s="6">
-        <f>C52/$G52*100</f>
+        <f t="shared" si="11"/>
         <v>3.0254802432915886</v>
       </c>
       <c r="W52" s="6">
-        <f>D52/$G52*100</f>
+        <f t="shared" si="12"/>
         <v>10.129595347363569</v>
       </c>
       <c r="X52" s="6">
-        <f>E52/$G52*100</f>
+        <f t="shared" si="13"/>
         <v>6.7880360802843209E-2</v>
       </c>
       <c r="Y52" s="6">
-        <f>F52/$G52*100</f>
+        <f t="shared" si="14"/>
         <v>1.8998079915232183E-2</v>
       </c>
       <c r="AC52">
@@ -42789,20 +42789,20 @@
         <v>1.856311209</v>
       </c>
       <c r="G53" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10526.345889208998</v>
       </c>
       <c r="H53" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11368.453560345719</v>
       </c>
       <c r="I53" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>232.48673840000001</v>
       </c>
-      <c r="J53" s="11"/>
+      <c r="J53" s="10"/>
       <c r="K53" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>48.89936363073739</v>
       </c>
       <c r="L53" s="6">
@@ -42829,25 +42829,25 @@
       <c r="S53" s="6">
         <v>76</v>
       </c>
-      <c r="T53" s="11"/>
+      <c r="T53" s="10"/>
       <c r="U53" s="6">
-        <f>B53/$G53*100</f>
+        <f t="shared" si="10"/>
         <v>87.018563672605282</v>
       </c>
       <c r="V53" s="6">
-        <f>C53/$G53*100</f>
+        <f t="shared" si="11"/>
         <v>2.9858276871008078</v>
       </c>
       <c r="W53" s="6">
-        <f>D53/$G53*100</f>
+        <f t="shared" si="12"/>
         <v>9.912942240190926</v>
       </c>
       <c r="X53" s="6">
-        <f>E53/$G53*100</f>
+        <f t="shared" si="13"/>
         <v>6.5031494044078014E-2</v>
       </c>
       <c r="Y53" s="6">
-        <f>F53/$G53*100</f>
+        <f t="shared" si="14"/>
         <v>1.7634906058929554E-2</v>
       </c>
       <c r="AC53">
@@ -42892,20 +42892,20 @@
         <v>1.856311209</v>
       </c>
       <c r="G54" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10526.345889208998</v>
       </c>
       <c r="H54" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11368.453560345719</v>
       </c>
       <c r="I54" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>233.92404590000001</v>
       </c>
-      <c r="J54" s="11"/>
+      <c r="J54" s="10"/>
       <c r="K54" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>48.598909601647406</v>
       </c>
       <c r="L54" s="6">
@@ -42926,25 +42926,25 @@
       <c r="S54" s="6">
         <v>76</v>
       </c>
-      <c r="T54" s="11"/>
+      <c r="T54" s="10"/>
       <c r="U54" s="6">
-        <f>B54/$G54*100</f>
+        <f t="shared" si="10"/>
         <v>87.018563672605282</v>
       </c>
       <c r="V54" s="6">
-        <f>C54/$G54*100</f>
+        <f t="shared" si="11"/>
         <v>2.9858276871008078</v>
       </c>
       <c r="W54" s="6">
-        <f>D54/$G54*100</f>
+        <f t="shared" si="12"/>
         <v>9.912942240190926</v>
       </c>
       <c r="X54" s="6">
-        <f>E54/$G54*100</f>
+        <f t="shared" si="13"/>
         <v>6.5031494044078014E-2</v>
       </c>
       <c r="Y54" s="6">
-        <f>F54/$G54*100</f>
+        <f t="shared" si="14"/>
         <v>1.7634906058929554E-2</v>
       </c>
       <c r="AC54">
@@ -42986,20 +42986,20 @@
         <v>1.856311209</v>
       </c>
       <c r="G55" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10526.345889208998</v>
       </c>
       <c r="H55" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11368.453560345719</v>
       </c>
       <c r="I55" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>235.2627057</v>
       </c>
-      <c r="J55" s="11"/>
+      <c r="J55" s="10"/>
       <c r="K55" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>48.322378706476464</v>
       </c>
       <c r="L55" s="6">
@@ -43020,25 +43020,25 @@
       <c r="S55" s="6">
         <v>76</v>
       </c>
-      <c r="T55" s="11"/>
+      <c r="T55" s="10"/>
       <c r="U55" s="6">
-        <f>B55/$G55*100</f>
+        <f t="shared" si="10"/>
         <v>87.018563672605282</v>
       </c>
       <c r="V55" s="6">
-        <f>C55/$G55*100</f>
+        <f t="shared" si="11"/>
         <v>2.9858276871008078</v>
       </c>
       <c r="W55" s="6">
-        <f>D55/$G55*100</f>
+        <f t="shared" si="12"/>
         <v>9.912942240190926</v>
       </c>
       <c r="X55" s="6">
-        <f>E55/$G55*100</f>
+        <f t="shared" si="13"/>
         <v>6.5031494044078014E-2</v>
       </c>
       <c r="Y55" s="6">
-        <f>F55/$G55*100</f>
+        <f t="shared" si="14"/>
         <v>1.7634906058929554E-2</v>
       </c>
       <c r="AC55">
@@ -43080,20 +43080,20 @@
         <v>1.856311209</v>
       </c>
       <c r="G56" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10526.345889208998</v>
       </c>
       <c r="H56" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11368.453560345719</v>
       </c>
       <c r="I56" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>236.51585300000002</v>
       </c>
-      <c r="J56" s="11"/>
+      <c r="J56" s="10"/>
       <c r="K56" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>48.066349109992714</v>
       </c>
       <c r="L56" s="6">
@@ -43114,25 +43114,25 @@
       <c r="S56" s="6">
         <v>76</v>
       </c>
-      <c r="T56" s="11"/>
+      <c r="T56" s="10"/>
       <c r="U56" s="6">
-        <f>B56/$G56*100</f>
+        <f t="shared" si="10"/>
         <v>87.018563672605282</v>
       </c>
       <c r="V56" s="6">
-        <f>C56/$G56*100</f>
+        <f t="shared" si="11"/>
         <v>2.9858276871008078</v>
       </c>
       <c r="W56" s="6">
-        <f>D56/$G56*100</f>
+        <f t="shared" si="12"/>
         <v>9.912942240190926</v>
       </c>
       <c r="X56" s="6">
-        <f>E56/$G56*100</f>
+        <f t="shared" si="13"/>
         <v>6.5031494044078014E-2</v>
       </c>
       <c r="Y56" s="6">
-        <f>F56/$G56*100</f>
+        <f t="shared" si="14"/>
         <v>1.7634906058929554E-2</v>
       </c>
       <c r="AC56">
@@ -43174,20 +43174,20 @@
         <v>1.856311209</v>
       </c>
       <c r="G57" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10526.345889208998</v>
       </c>
       <c r="H57" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11368.453560345719</v>
       </c>
       <c r="I57" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>237.69413579999997</v>
       </c>
-      <c r="J57" s="11"/>
+      <c r="J57" s="10"/>
       <c r="K57" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>47.828077550517847</v>
       </c>
       <c r="L57" s="6">
@@ -43208,25 +43208,25 @@
       <c r="S57" s="6">
         <v>76</v>
       </c>
-      <c r="T57" s="11"/>
+      <c r="T57" s="10"/>
       <c r="U57" s="6">
-        <f>B57/$G57*100</f>
+        <f t="shared" si="10"/>
         <v>87.018563672605282</v>
       </c>
       <c r="V57" s="6">
-        <f>C57/$G57*100</f>
+        <f t="shared" si="11"/>
         <v>2.9858276871008078</v>
       </c>
       <c r="W57" s="6">
-        <f>D57/$G57*100</f>
+        <f t="shared" si="12"/>
         <v>9.912942240190926</v>
       </c>
       <c r="X57" s="6">
-        <f>E57/$G57*100</f>
+        <f t="shared" si="13"/>
         <v>6.5031494044078014E-2</v>
       </c>
       <c r="Y57" s="6">
-        <f>F57/$G57*100</f>
+        <f t="shared" si="14"/>
         <v>1.7634906058929554E-2</v>
       </c>
       <c r="AC57">
@@ -43268,20 +43268,20 @@
         <v>1.856311209</v>
       </c>
       <c r="G58" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10526.345889208998</v>
       </c>
       <c r="H58" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11368.453560345719</v>
       </c>
       <c r="I58" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>238.80630870000002</v>
       </c>
-      <c r="J58" s="11"/>
+      <c r="J58" s="10"/>
       <c r="K58" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>47.605331794761412</v>
       </c>
       <c r="L58" s="6">
@@ -43302,25 +43302,25 @@
       <c r="S58" s="6">
         <v>76</v>
       </c>
-      <c r="T58" s="11"/>
+      <c r="T58" s="10"/>
       <c r="U58" s="6">
-        <f>B58/$G58*100</f>
+        <f t="shared" si="10"/>
         <v>87.018563672605282</v>
       </c>
       <c r="V58" s="6">
-        <f>C58/$G58*100</f>
+        <f t="shared" si="11"/>
         <v>2.9858276871008078</v>
       </c>
       <c r="W58" s="6">
-        <f>D58/$G58*100</f>
+        <f t="shared" si="12"/>
         <v>9.912942240190926</v>
       </c>
       <c r="X58" s="6">
-        <f>E58/$G58*100</f>
+        <f t="shared" si="13"/>
         <v>6.5031494044078014E-2</v>
       </c>
       <c r="Y58" s="6">
-        <f>F58/$G58*100</f>
+        <f t="shared" si="14"/>
         <v>1.7634906058929554E-2</v>
       </c>
       <c r="AC58">
@@ -43365,20 +43365,20 @@
         <v>1.856311209</v>
       </c>
       <c r="G59" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10526.345889208998</v>
       </c>
       <c r="H59" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11368.453560345719</v>
       </c>
       <c r="I59" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>239.85965880000001</v>
       </c>
-      <c r="J59" s="11"/>
+      <c r="J59" s="10"/>
       <c r="K59" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>47.396271708303281</v>
       </c>
       <c r="L59" s="6">
@@ -43399,25 +43399,25 @@
       <c r="S59" s="6">
         <v>76</v>
       </c>
-      <c r="T59" s="11"/>
+      <c r="T59" s="10"/>
       <c r="U59" s="6">
-        <f>B59/$G59*100</f>
+        <f t="shared" si="10"/>
         <v>87.018563672605282</v>
       </c>
       <c r="V59" s="6">
-        <f>C59/$G59*100</f>
+        <f t="shared" si="11"/>
         <v>2.9858276871008078</v>
       </c>
       <c r="W59" s="6">
-        <f>D59/$G59*100</f>
+        <f t="shared" si="12"/>
         <v>9.912942240190926</v>
       </c>
       <c r="X59" s="6">
-        <f>E59/$G59*100</f>
+        <f t="shared" si="13"/>
         <v>6.5031494044078014E-2</v>
       </c>
       <c r="Y59" s="6">
-        <f>F59/$G59*100</f>
+        <f t="shared" si="14"/>
         <v>1.7634906058929554E-2</v>
       </c>
       <c r="AC59">
@@ -43459,20 +43459,20 @@
         <v>1.856311209</v>
       </c>
       <c r="G60" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10526.345889208998</v>
       </c>
       <c r="H60" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11368.453560345719</v>
       </c>
       <c r="I60" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>240.86031829999999</v>
       </c>
-      <c r="J60" s="11"/>
+      <c r="J60" s="10"/>
       <c r="K60" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>47.199362853062041</v>
       </c>
       <c r="L60" s="6">
@@ -43493,25 +43493,25 @@
       <c r="S60" s="6">
         <v>76</v>
       </c>
-      <c r="T60" s="11"/>
+      <c r="T60" s="10"/>
       <c r="U60" s="6">
-        <f>B60/$G60*100</f>
+        <f t="shared" si="10"/>
         <v>87.018563672605282</v>
       </c>
       <c r="V60" s="6">
-        <f>C60/$G60*100</f>
+        <f t="shared" si="11"/>
         <v>2.9858276871008078</v>
       </c>
       <c r="W60" s="6">
-        <f>D60/$G60*100</f>
+        <f t="shared" si="12"/>
         <v>9.912942240190926</v>
       </c>
       <c r="X60" s="6">
-        <f>E60/$G60*100</f>
+        <f t="shared" si="13"/>
         <v>6.5031494044078014E-2</v>
       </c>
       <c r="Y60" s="6">
-        <f>F60/$G60*100</f>
+        <f t="shared" si="14"/>
         <v>1.7634906058929554E-2</v>
       </c>
       <c r="AC60">
@@ -43553,20 +43553,20 @@
         <v>1.856311209</v>
       </c>
       <c r="G61" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10526.345889208998</v>
       </c>
       <c r="H61" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11368.453560345719</v>
       </c>
       <c r="I61" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>241.81349740000002</v>
       </c>
-      <c r="J61" s="11"/>
+      <c r="J61" s="10"/>
       <c r="K61" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>47.013312666912029</v>
       </c>
       <c r="L61" s="6">
@@ -43587,25 +43587,25 @@
       <c r="S61" s="6">
         <v>76</v>
       </c>
-      <c r="T61" s="11"/>
+      <c r="T61" s="10"/>
       <c r="U61" s="6">
-        <f>B61/$G61*100</f>
+        <f t="shared" si="10"/>
         <v>87.018563672605282</v>
       </c>
       <c r="V61" s="6">
-        <f>C61/$G61*100</f>
+        <f t="shared" si="11"/>
         <v>2.9858276871008078</v>
       </c>
       <c r="W61" s="6">
-        <f>D61/$G61*100</f>
+        <f t="shared" si="12"/>
         <v>9.912942240190926</v>
       </c>
       <c r="X61" s="6">
-        <f>E61/$G61*100</f>
+        <f t="shared" si="13"/>
         <v>6.5031494044078014E-2</v>
       </c>
       <c r="Y61" s="6">
-        <f>F61/$G61*100</f>
+        <f t="shared" si="14"/>
         <v>1.7634906058929554E-2</v>
       </c>
       <c r="AC61">
@@ -43647,20 +43647,20 @@
         <v>1.856311209</v>
       </c>
       <c r="G62" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10526.345889208998</v>
       </c>
       <c r="H62" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11368.453560345719</v>
       </c>
       <c r="I62" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>242.72366120000004</v>
       </c>
-      <c r="J62" s="11"/>
+      <c r="J62" s="10"/>
       <c r="K62" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>46.837022415290257</v>
       </c>
       <c r="L62" s="6">
@@ -43681,25 +43681,25 @@
       <c r="S62" s="6">
         <v>76</v>
       </c>
-      <c r="T62" s="11"/>
+      <c r="T62" s="10"/>
       <c r="U62" s="6">
-        <f>B62/$G62*100</f>
+        <f t="shared" si="10"/>
         <v>87.018563672605282</v>
       </c>
       <c r="V62" s="6">
-        <f>C62/$G62*100</f>
+        <f t="shared" si="11"/>
         <v>2.9858276871008078</v>
       </c>
       <c r="W62" s="6">
-        <f>D62/$G62*100</f>
+        <f t="shared" si="12"/>
         <v>9.912942240190926</v>
       </c>
       <c r="X62" s="6">
-        <f>E62/$G62*100</f>
+        <f t="shared" si="13"/>
         <v>6.5031494044078014E-2</v>
       </c>
       <c r="Y62" s="6">
-        <f>F62/$G62*100</f>
+        <f t="shared" si="14"/>
         <v>1.7634906058929554E-2</v>
       </c>
       <c r="AC62">
@@ -43741,20 +43741,20 @@
         <v>1.856311209</v>
       </c>
       <c r="G63" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10526.345889208998</v>
       </c>
       <c r="H63" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11368.453560345719</v>
       </c>
       <c r="I63" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>243.59466650000002</v>
       </c>
-      <c r="J63" s="11"/>
+      <c r="J63" s="10"/>
       <c r="K63" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>46.669550379280238</v>
       </c>
       <c r="L63" s="6">
@@ -43775,25 +43775,25 @@
       <c r="S63" s="6">
         <v>76</v>
       </c>
-      <c r="T63" s="11"/>
+      <c r="T63" s="10"/>
       <c r="U63" s="6">
-        <f>B63/$G63*100</f>
+        <f t="shared" si="10"/>
         <v>87.018563672605282</v>
       </c>
       <c r="V63" s="6">
-        <f>C63/$G63*100</f>
+        <f t="shared" si="11"/>
         <v>2.9858276871008078</v>
       </c>
       <c r="W63" s="6">
-        <f>D63/$G63*100</f>
+        <f t="shared" si="12"/>
         <v>9.912942240190926</v>
       </c>
       <c r="X63" s="6">
-        <f>E63/$G63*100</f>
+        <f t="shared" si="13"/>
         <v>6.5031494044078014E-2</v>
       </c>
       <c r="Y63" s="6">
-        <f>F63/$G63*100</f>
+        <f t="shared" si="14"/>
         <v>1.7634906058929554E-2</v>
       </c>
       <c r="AC63">
@@ -43838,20 +43838,20 @@
         <v>1.856311209</v>
       </c>
       <c r="G64" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10526.345889208998</v>
       </c>
       <c r="H64" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11368.453560345719</v>
       </c>
       <c r="I64" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>244.42986730000001</v>
       </c>
-      <c r="J64" s="11"/>
+      <c r="J64" s="10"/>
       <c r="K64" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>46.510083591350536</v>
       </c>
       <c r="L64" s="6">
@@ -43872,25 +43872,25 @@
       <c r="S64" s="6">
         <v>76</v>
       </c>
-      <c r="T64" s="11"/>
+      <c r="T64" s="10"/>
       <c r="U64" s="6">
-        <f>B64/$G64*100</f>
+        <f t="shared" si="10"/>
         <v>87.018563672605282</v>
       </c>
       <c r="V64" s="6">
-        <f>C64/$G64*100</f>
+        <f t="shared" si="11"/>
         <v>2.9858276871008078</v>
       </c>
       <c r="W64" s="6">
-        <f>D64/$G64*100</f>
+        <f t="shared" si="12"/>
         <v>9.912942240190926</v>
       </c>
       <c r="X64" s="6">
-        <f>E64/$G64*100</f>
+        <f t="shared" si="13"/>
         <v>6.5031494044078014E-2</v>
       </c>
       <c r="Y64" s="6">
-        <f>F64/$G64*100</f>
+        <f t="shared" si="14"/>
         <v>1.7634906058929554E-2</v>
       </c>
       <c r="AC64">
@@ -43932,20 +43932,20 @@
         <v>1.856311209</v>
       </c>
       <c r="G65" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10526.345889208998</v>
       </c>
       <c r="H65" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11368.453560345719</v>
       </c>
       <c r="I65" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>245.23219999999998</v>
       </c>
-      <c r="J65" s="11"/>
+      <c r="J65" s="10"/>
       <c r="K65" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>46.357915315956554</v>
       </c>
       <c r="L65" s="6">
@@ -43966,25 +43966,25 @@
       <c r="S65" s="6">
         <v>76</v>
       </c>
-      <c r="T65" s="11"/>
+      <c r="T65" s="10"/>
       <c r="U65" s="6">
-        <f>B65/$G65*100</f>
+        <f t="shared" si="10"/>
         <v>87.018563672605282</v>
       </c>
       <c r="V65" s="6">
-        <f>C65/$G65*100</f>
+        <f t="shared" si="11"/>
         <v>2.9858276871008078</v>
       </c>
       <c r="W65" s="6">
-        <f>D65/$G65*100</f>
+        <f t="shared" si="12"/>
         <v>9.912942240190926</v>
       </c>
       <c r="X65" s="6">
-        <f>E65/$G65*100</f>
+        <f t="shared" si="13"/>
         <v>6.5031494044078014E-2</v>
       </c>
       <c r="Y65" s="6">
-        <f>F65/$G65*100</f>
+        <f t="shared" si="14"/>
         <v>1.7634906058929554E-2</v>
       </c>
       <c r="AC65">
@@ -44026,20 +44026,20 @@
         <v>1.856311209</v>
       </c>
       <c r="G66" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10526.345889208998</v>
       </c>
       <c r="H66" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11368.453560345719</v>
       </c>
       <c r="I66" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>246.00424960000001</v>
       </c>
-      <c r="J66" s="11"/>
+      <c r="J66" s="10"/>
       <c r="K66" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>46.212427544770833</v>
       </c>
       <c r="L66" s="6">
@@ -44060,25 +44060,25 @@
       <c r="S66" s="6">
         <v>76</v>
       </c>
-      <c r="T66" s="11"/>
+      <c r="T66" s="10"/>
       <c r="U66" s="6">
-        <f>B66/$G66*100</f>
+        <f t="shared" si="10"/>
         <v>87.018563672605282</v>
       </c>
       <c r="V66" s="6">
-        <f>C66/$G66*100</f>
+        <f t="shared" si="11"/>
         <v>2.9858276871008078</v>
       </c>
       <c r="W66" s="6">
-        <f>D66/$G66*100</f>
+        <f t="shared" si="12"/>
         <v>9.912942240190926</v>
       </c>
       <c r="X66" s="6">
-        <f>E66/$G66*100</f>
+        <f t="shared" si="13"/>
         <v>6.5031494044078014E-2</v>
       </c>
       <c r="Y66" s="6">
-        <f>F66/$G66*100</f>
+        <f t="shared" si="14"/>
         <v>1.7634906058929554E-2</v>
       </c>
       <c r="AC66">
@@ -44120,20 +44120,20 @@
         <v>1.856311209</v>
       </c>
       <c r="G67" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10526.345889208998</v>
       </c>
       <c r="H67" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11368.453560345719</v>
       </c>
       <c r="I67" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>246.74830409999998</v>
       </c>
-      <c r="J67" s="11"/>
+      <c r="J67" s="10"/>
       <c r="K67" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>46.073076780857676</v>
       </c>
       <c r="L67" s="6">
@@ -44154,25 +44154,25 @@
       <c r="S67" s="6">
         <v>76</v>
       </c>
-      <c r="T67" s="11"/>
+      <c r="T67" s="10"/>
       <c r="U67" s="6">
-        <f>B67/$G67*100</f>
+        <f t="shared" si="10"/>
         <v>87.018563672605282</v>
       </c>
       <c r="V67" s="6">
-        <f>C67/$G67*100</f>
+        <f t="shared" si="11"/>
         <v>2.9858276871008078</v>
       </c>
       <c r="W67" s="6">
-        <f>D67/$G67*100</f>
+        <f t="shared" si="12"/>
         <v>9.912942240190926</v>
       </c>
       <c r="X67" s="6">
-        <f>E67/$G67*100</f>
+        <f t="shared" si="13"/>
         <v>6.5031494044078014E-2</v>
       </c>
       <c r="Y67" s="6">
-        <f>F67/$G67*100</f>
+        <f t="shared" si="14"/>
         <v>1.7634906058929554E-2</v>
       </c>
       <c r="AC67">
@@ -44214,20 +44214,20 @@
         <v>1.856311209</v>
       </c>
       <c r="G68" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10526.345889208998</v>
       </c>
       <c r="H68" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11368.453560345719</v>
       </c>
       <c r="I68" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>247.46639890000003</v>
       </c>
-      <c r="J68" s="11"/>
+      <c r="J68" s="10"/>
       <c r="K68" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>45.93938252174452</v>
       </c>
       <c r="L68" s="6">
@@ -44248,25 +44248,25 @@
       <c r="S68" s="6">
         <v>76</v>
       </c>
-      <c r="T68" s="11"/>
+      <c r="T68" s="10"/>
       <c r="U68" s="6">
-        <f>B68/$G68*100</f>
+        <f t="shared" si="10"/>
         <v>87.018563672605282</v>
       </c>
       <c r="V68" s="6">
-        <f>C68/$G68*100</f>
+        <f t="shared" si="11"/>
         <v>2.9858276871008078</v>
       </c>
       <c r="W68" s="6">
-        <f>D68/$G68*100</f>
+        <f t="shared" si="12"/>
         <v>9.912942240190926</v>
       </c>
       <c r="X68" s="6">
-        <f>E68/$G68*100</f>
+        <f t="shared" si="13"/>
         <v>6.5031494044078014E-2</v>
       </c>
       <c r="Y68" s="6">
-        <f>F68/$G68*100</f>
+        <f t="shared" si="14"/>
         <v>1.7634906058929554E-2</v>
       </c>
       <c r="AC68">
@@ -44311,20 +44311,20 @@
         <v>1.856311209</v>
       </c>
       <c r="G69" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10526.345889208998</v>
       </c>
       <c r="H69" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11368.453560345719</v>
       </c>
       <c r="I69" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>248.16035240000002</v>
       </c>
-      <c r="J69" s="11"/>
+      <c r="J69" s="10"/>
       <c r="K69" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>45.810918022961822</v>
       </c>
       <c r="L69" s="6">
@@ -44345,25 +44345,25 @@
       <c r="S69" s="6">
         <v>76</v>
       </c>
-      <c r="T69" s="11"/>
+      <c r="T69" s="10"/>
       <c r="U69" s="6">
-        <f>B69/$G69*100</f>
+        <f t="shared" si="10"/>
         <v>87.018563672605282</v>
       </c>
       <c r="V69" s="6">
-        <f>C69/$G69*100</f>
+        <f t="shared" si="11"/>
         <v>2.9858276871008078</v>
       </c>
       <c r="W69" s="6">
-        <f>D69/$G69*100</f>
+        <f t="shared" si="12"/>
         <v>9.912942240190926</v>
       </c>
       <c r="X69" s="6">
-        <f>E69/$G69*100</f>
+        <f t="shared" si="13"/>
         <v>6.5031494044078014E-2</v>
       </c>
       <c r="Y69" s="6">
-        <f>F69/$G69*100</f>
+        <f t="shared" si="14"/>
         <v>1.7634906058929554E-2</v>
       </c>
       <c r="AC69">
@@ -44405,20 +44405,20 @@
         <v>1.856311209</v>
       </c>
       <c r="G70" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10526.345889208998</v>
       </c>
       <c r="H70" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11368.453560345719</v>
       </c>
       <c r="I70" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>248.83179619999999</v>
       </c>
-      <c r="J70" s="11"/>
+      <c r="J70" s="10"/>
       <c r="K70" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>45.687302563247421</v>
       </c>
       <c r="L70" s="6">
@@ -44439,25 +44439,25 @@
       <c r="S70" s="6">
         <v>76</v>
       </c>
-      <c r="T70" s="11"/>
+      <c r="T70" s="10"/>
       <c r="U70" s="6">
-        <f>B70/$G70*100</f>
+        <f t="shared" si="10"/>
         <v>87.018563672605282</v>
       </c>
       <c r="V70" s="6">
-        <f>C70/$G70*100</f>
+        <f t="shared" si="11"/>
         <v>2.9858276871008078</v>
       </c>
       <c r="W70" s="6">
-        <f>D70/$G70*100</f>
+        <f t="shared" si="12"/>
         <v>9.912942240190926</v>
       </c>
       <c r="X70" s="6">
-        <f>E70/$G70*100</f>
+        <f t="shared" si="13"/>
         <v>6.5031494044078014E-2</v>
       </c>
       <c r="Y70" s="6">
-        <f>F70/$G70*100</f>
+        <f t="shared" si="14"/>
         <v>1.7634906058929554E-2</v>
       </c>
       <c r="AC70">
@@ -44499,20 +44499,20 @@
         <v>1.856311209</v>
       </c>
       <c r="G71" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10526.345889208998</v>
       </c>
       <c r="H71" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11368.453560345719</v>
       </c>
       <c r="I71" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>249.4822001</v>
       </c>
-      <c r="J71" s="11"/>
+      <c r="J71" s="10"/>
       <c r="K71" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>45.56819506878206</v>
       </c>
       <c r="L71" s="6">
@@ -44533,25 +44533,25 @@
       <c r="S71" s="6">
         <v>76</v>
       </c>
-      <c r="T71" s="11"/>
+      <c r="T71" s="10"/>
       <c r="U71" s="6">
-        <f>B71/$G71*100</f>
+        <f t="shared" si="10"/>
         <v>87.018563672605282</v>
       </c>
       <c r="V71" s="6">
-        <f>C71/$G71*100</f>
+        <f t="shared" si="11"/>
         <v>2.9858276871008078</v>
       </c>
       <c r="W71" s="6">
-        <f>D71/$G71*100</f>
+        <f t="shared" si="12"/>
         <v>9.912942240190926</v>
       </c>
       <c r="X71" s="6">
-        <f>E71/$G71*100</f>
+        <f t="shared" si="13"/>
         <v>6.5031494044078014E-2</v>
       </c>
       <c r="Y71" s="6">
-        <f>F71/$G71*100</f>
+        <f t="shared" si="14"/>
         <v>1.7634906058929554E-2</v>
       </c>
       <c r="AC71">
@@ -44593,20 +44593,20 @@
         <v>1.856311209</v>
       </c>
       <c r="G72" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10526.345889208998</v>
       </c>
       <c r="H72" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11368.453560345719</v>
       </c>
       <c r="I72" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>250.11289269999997</v>
       </c>
-      <c r="J72" s="11"/>
+      <c r="J72" s="10"/>
       <c r="K72" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>45.453288863368215</v>
       </c>
       <c r="L72" s="6">
@@ -44627,25 +44627,25 @@
       <c r="S72" s="6">
         <v>76</v>
       </c>
-      <c r="T72" s="11"/>
+      <c r="T72" s="10"/>
       <c r="U72" s="6">
-        <f>B72/$G72*100</f>
+        <f t="shared" si="10"/>
         <v>87.018563672605282</v>
       </c>
       <c r="V72" s="6">
-        <f>C72/$G72*100</f>
+        <f t="shared" si="11"/>
         <v>2.9858276871008078</v>
       </c>
       <c r="W72" s="6">
-        <f>D72/$G72*100</f>
+        <f t="shared" si="12"/>
         <v>9.912942240190926</v>
       </c>
       <c r="X72" s="6">
-        <f>E72/$G72*100</f>
+        <f t="shared" si="13"/>
         <v>6.5031494044078014E-2</v>
       </c>
       <c r="Y72" s="6">
-        <f>F72/$G72*100</f>
+        <f t="shared" si="14"/>
         <v>1.7634906058929554E-2</v>
       </c>
       <c r="AC72">
@@ -44687,20 +44687,20 @@
         <v>1.856311209</v>
       </c>
       <c r="G73" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10526.345889208998</v>
       </c>
       <c r="H73" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11368.453560345719</v>
       </c>
       <c r="I73" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>250.72507910000002</v>
       </c>
-      <c r="J73" s="11"/>
+      <c r="J73" s="10"/>
       <c r="K73" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>45.342307204184735</v>
       </c>
       <c r="L73" s="6">
@@ -44723,25 +44723,25 @@
       <c r="S73" s="6">
         <v>76</v>
       </c>
-      <c r="T73" s="11"/>
+      <c r="T73" s="10"/>
       <c r="U73" s="6">
-        <f>B73/$G73*100</f>
+        <f t="shared" si="10"/>
         <v>87.018563672605282</v>
       </c>
       <c r="V73" s="6">
-        <f>C73/$G73*100</f>
+        <f t="shared" si="11"/>
         <v>2.9858276871008078</v>
       </c>
       <c r="W73" s="6">
-        <f>D73/$G73*100</f>
+        <f t="shared" si="12"/>
         <v>9.912942240190926</v>
       </c>
       <c r="X73" s="6">
-        <f>E73/$G73*100</f>
+        <f t="shared" si="13"/>
         <v>6.5031494044078014E-2</v>
       </c>
       <c r="Y73" s="6">
-        <f>F73/$G73*100</f>
+        <f t="shared" si="14"/>
         <v>1.7634906058929554E-2</v>
       </c>
       <c r="AC73">
@@ -44796,19 +44796,19 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -49482,28 +49482,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AF334EA-9A50-43B1-8DC3-AE424E8C06D6}">
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S1" sqref="S1"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -49574,7 +49574,7 @@
         <v>1996</v>
       </c>
       <c r="B4">
-        <v>99.666666699999993</v>
+        <v>99.6666666666666</v>
       </c>
       <c r="H4">
         <v>92</v>
@@ -49591,7 +49591,7 @@
         <v>1997</v>
       </c>
       <c r="B5">
-        <v>99.333333300000007</v>
+        <v>99.3333333333333</v>
       </c>
       <c r="H5">
         <v>92</v>
@@ -49628,7 +49628,7 @@
         <v>1999</v>
       </c>
       <c r="B7">
-        <v>98.166666700000007</v>
+        <v>98.1666666666666</v>
       </c>
       <c r="H7">
         <v>92</v>
@@ -49645,7 +49645,7 @@
         <v>2000</v>
       </c>
       <c r="B8">
-        <v>97.333333300000007</v>
+        <v>97.3333333333333</v>
       </c>
       <c r="H8">
         <v>92</v>
@@ -49691,7 +49691,7 @@
         <v>2002</v>
       </c>
       <c r="B10">
-        <v>95.666666700000007</v>
+        <v>95.6666666666666</v>
       </c>
       <c r="H10">
         <v>92</v>
@@ -49714,7 +49714,7 @@
         <v>2003</v>
       </c>
       <c r="B11">
-        <v>94.833333300000007</v>
+        <v>94.8333333333333</v>
       </c>
       <c r="H11">
         <v>92</v>
@@ -49763,7 +49763,7 @@
         <v>2005</v>
       </c>
       <c r="B13">
-        <v>86.082000000000008</v>
+        <v>93.768129340000002</v>
       </c>
       <c r="H13">
         <v>92</v>
@@ -49786,7 +49786,7 @@
         <v>2006</v>
       </c>
       <c r="B14">
-        <v>78.164000000000001</v>
+        <v>93.536258679999989</v>
       </c>
       <c r="H14">
         <v>92</v>
@@ -49809,7 +49809,7 @@
         <v>2007</v>
       </c>
       <c r="B15">
-        <v>70.245999999999995</v>
+        <v>93.30438801999999</v>
       </c>
       <c r="H15">
         <v>92</v>
@@ -49832,7 +49832,7 @@
         <v>2008</v>
       </c>
       <c r="B16">
-        <v>62.327999999999996</v>
+        <v>93.072517359999992</v>
       </c>
       <c r="H16">
         <v>92</v>
@@ -49858,7 +49858,7 @@
         <v>2009</v>
       </c>
       <c r="B17">
-        <v>54.410000000000004</v>
+        <v>92.840646699999994</v>
       </c>
       <c r="C17">
         <v>54.410000000000004</v>
@@ -49887,7 +49887,7 @@
         <v>2010</v>
       </c>
       <c r="B18">
-        <v>34.29</v>
+        <v>84.828496000000001</v>
       </c>
       <c r="C18">
         <v>34.29</v>
@@ -49916,7 +49916,7 @@
         <v>2011</v>
       </c>
       <c r="B19">
-        <v>75.63</v>
+        <v>92.755418000000006</v>
       </c>
       <c r="C19">
         <v>75.63</v>
@@ -49945,7 +49945,7 @@
         <v>2012</v>
       </c>
       <c r="B20">
-        <v>75.11</v>
+        <v>90.832328099999899</v>
       </c>
       <c r="C20">
         <v>75.11</v>
@@ -49974,7 +49974,7 @@
         <v>2013</v>
       </c>
       <c r="B21">
-        <v>63.019999999999996</v>
+        <v>84.717097199999998</v>
       </c>
       <c r="C21">
         <v>63.019999999999996</v>
@@ -50003,7 +50003,7 @@
         <v>2014</v>
       </c>
       <c r="B22">
-        <v>29.98</v>
+        <v>59.613632199999998</v>
       </c>
       <c r="C22">
         <v>29.98</v>
@@ -50032,7 +50032,7 @@
         <v>2015</v>
       </c>
       <c r="B23">
-        <v>81.069999999999993</v>
+        <v>91.116584599999996</v>
       </c>
       <c r="C23">
         <v>81.069999999999993</v>
@@ -50058,7 +50058,7 @@
         <v>2016</v>
       </c>
       <c r="B24">
-        <v>77.02</v>
+        <v>85.439676300000002</v>
       </c>
       <c r="C24">
         <v>77.02</v>
@@ -50084,7 +50084,7 @@
         <v>2017</v>
       </c>
       <c r="B25">
-        <v>76.92</v>
+        <v>89.2007105</v>
       </c>
       <c r="C25">
         <v>76.92</v>
@@ -50110,7 +50110,7 @@
         <v>2018</v>
       </c>
       <c r="B26">
-        <v>72.27</v>
+        <v>87.078198799999996</v>
       </c>
       <c r="C26">
         <v>72.27</v>
@@ -50133,7 +50133,7 @@
         <v>2019</v>
       </c>
       <c r="B27">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H27">
         <v>92</v>
@@ -50150,7 +50150,7 @@
         <v>2020</v>
       </c>
       <c r="B28">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="G28">
         <v>73.3</v>
@@ -50170,7 +50170,7 @@
         <v>2021</v>
       </c>
       <c r="B29">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H29">
         <v>92</v>
@@ -50184,7 +50184,7 @@
         <v>2022</v>
       </c>
       <c r="B30">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H30">
         <v>92</v>
@@ -50198,7 +50198,7 @@
         <v>2023</v>
       </c>
       <c r="B31">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H31">
         <v>92</v>
@@ -50212,7 +50212,7 @@
         <v>2024</v>
       </c>
       <c r="B32">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H32">
         <v>92</v>
@@ -50226,7 +50226,7 @@
         <v>2025</v>
       </c>
       <c r="B33">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H33">
         <v>92</v>
@@ -50240,7 +50240,7 @@
         <v>2026</v>
       </c>
       <c r="B34">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H34">
         <v>92</v>
@@ -50254,7 +50254,7 @@
         <v>2027</v>
       </c>
       <c r="B35">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H35">
         <v>92</v>
@@ -50268,7 +50268,7 @@
         <v>2028</v>
       </c>
       <c r="B36">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H36">
         <v>92</v>
@@ -50282,7 +50282,7 @@
         <v>2029</v>
       </c>
       <c r="B37">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H37">
         <v>92</v>
@@ -50296,7 +50296,7 @@
         <v>2030</v>
       </c>
       <c r="B38">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="G38">
         <v>44.8</v>
@@ -50316,7 +50316,7 @@
         <v>2031</v>
       </c>
       <c r="B39">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H39">
         <v>92</v>
@@ -50330,7 +50330,7 @@
         <v>2032</v>
       </c>
       <c r="B40">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H40">
         <v>92</v>
@@ -50344,7 +50344,7 @@
         <v>2033</v>
       </c>
       <c r="B41">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H41">
         <v>92</v>
@@ -50358,7 +50358,7 @@
         <v>2034</v>
       </c>
       <c r="B42">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H42">
         <v>92</v>
@@ -50372,7 +50372,7 @@
         <v>2035</v>
       </c>
       <c r="B43">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H43">
         <v>92</v>
@@ -50386,7 +50386,7 @@
         <v>2036</v>
       </c>
       <c r="B44">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H44">
         <v>92</v>
@@ -50400,7 +50400,7 @@
         <v>2037</v>
       </c>
       <c r="B45">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H45">
         <v>92</v>
@@ -50414,7 +50414,7 @@
         <v>2038</v>
       </c>
       <c r="B46">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H46">
         <v>92</v>
@@ -50428,7 +50428,7 @@
         <v>2039</v>
       </c>
       <c r="B47">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H47">
         <v>92</v>
@@ -50442,7 +50442,7 @@
         <v>2040</v>
       </c>
       <c r="B48">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H48">
         <v>92</v>
@@ -50456,7 +50456,7 @@
         <v>2041</v>
       </c>
       <c r="B49">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H49">
         <v>92</v>
@@ -50470,7 +50470,7 @@
         <v>2042</v>
       </c>
       <c r="B50">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H50">
         <v>92</v>
@@ -50484,7 +50484,7 @@
         <v>2043</v>
       </c>
       <c r="B51">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H51">
         <v>92</v>
@@ -50498,7 +50498,7 @@
         <v>2044</v>
       </c>
       <c r="B52">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H52">
         <v>92</v>
@@ -50512,7 +50512,7 @@
         <v>2045</v>
       </c>
       <c r="B53">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H53">
         <v>92</v>
@@ -50526,7 +50526,7 @@
         <v>2046</v>
       </c>
       <c r="B54">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H54">
         <v>92</v>
@@ -50540,7 +50540,7 @@
         <v>2047</v>
       </c>
       <c r="B55">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H55">
         <v>92</v>
@@ -50554,7 +50554,7 @@
         <v>2048</v>
       </c>
       <c r="B56">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H56">
         <v>92</v>
@@ -50568,7 +50568,7 @@
         <v>2049</v>
       </c>
       <c r="B57">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H57">
         <v>92</v>
@@ -50582,7 +50582,7 @@
         <v>2050</v>
       </c>
       <c r="B58">
-        <v>72.27</v>
+        <v>81.800867599999904</v>
       </c>
       <c r="H58">
         <v>92</v>

</xml_diff>

<commit_message>
Fixed bug in lifetime vs recycling journal
and a few other tweaks
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/SupportingMaterial/BaselineGraphs.xlsx
+++ b/PV_ICE/baselines/SupportingMaterial/BaselineGraphs.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E714B69F-5F21-410D-8D67-8BB966FB66B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFF3533-1044-47DA-9A33-78EC85D71F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{31D47E9D-A833-4D35-B79A-EFF0E4DE6D01}"/>
+    <workbookView xWindow="28680" yWindow="-2340" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{31D47E9D-A833-4D35-B79A-EFF0E4DE6D01}"/>
   </bookViews>
   <sheets>
     <sheet name="mass per m2" sheetId="1" r:id="rId1"/>
     <sheet name="VirginMatEff" sheetId="5" r:id="rId2"/>
     <sheet name="MFG Eff" sheetId="3" r:id="rId3"/>
     <sheet name="SF-all on one" sheetId="2" r:id="rId4"/>
+    <sheet name="ModuleLifetime" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="48">
   <si>
     <t>Year</t>
   </si>
@@ -166,6 +167,21 @@
   </si>
   <si>
     <t>Backsheet</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>Module Efficiency</t>
+  </si>
+  <si>
+    <t>Economic Lifetime</t>
+  </si>
+  <si>
+    <t>[%]</t>
+  </si>
+  <si>
+    <t>[years]</t>
   </si>
 </sst>
 </file>
@@ -13131,6 +13147,2005 @@
     <a:p>
       <a:pPr>
         <a:defRPr sz="1400">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+          <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Properties </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>of Historical PV Modules and </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Current Technology Trends</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.5698844759667903E-2"/>
+          <c:y val="8.4891651624061246E-2"/>
+          <c:w val="0.8068869305743015"/>
+          <c:h val="0.83475559964786761"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ModuleLifetime!$B$1:$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Module Efficiency</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>[%]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ModuleLifetime!$A$18:$A$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2041</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2042</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2043</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2044</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2046</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2047</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ModuleLifetime!$B$18:$B$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>14.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20.921698800000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21.480425369999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>21.88587403</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22.205627280000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>22.470349479999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22.6966295</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>22.894483210000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>23.070433690000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>23.228972280000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>23.373326200000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>23.505894179999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23.62850877</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23.742602300000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>23.849315969999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>23.949574089999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>24.044135990000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>24.133633240000002</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>24.218596949999998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>24.299478069999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>24.376662799999998</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>24.450484530000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>24.52123306</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>24.589161900000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>24.654494150000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>24.717427180000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>24.778136459999999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>24.8367787</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>24.893494459999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>24.94841027</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>25.001640479999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CBE7-4BA7-88C4-1849B8EEB50E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ModuleLifetime!$F$1:$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Economic Lifetime</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>[years]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ModuleLifetime!$A$18:$A$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2041</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2042</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2043</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2044</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2046</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2047</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ModuleLifetime!$F$18:$F$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>22.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-CBE7-4BA7-88C4-1849B8EEB50E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ModuleLifetime!$C$1:$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>T50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>[years]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ModuleLifetime!$A$18:$A$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2041</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2042</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2043</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2044</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2046</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2047</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ModuleLifetime!$C$18:$C$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CBE7-4BA7-88C4-1849B8EEB50E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ModuleLifetime!$D$1:$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>T90</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>[years]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ModuleLifetime!$A$18:$A$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2041</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2042</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2043</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2044</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2046</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2047</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ModuleLifetime!$D$18:$D$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-CBE7-4BA7-88C4-1849B8EEB50E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="551222288"/>
+        <c:axId val="551219664"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ModuleLifetime!$E$1:$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Degradation Rate</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>[%]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ModuleLifetime!$A$18:$A$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2041</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2042</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2043</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2044</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2046</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2047</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ModuleLifetime!$E$18:$E$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-CBE7-4BA7-88C4-1849B8EEB50E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="545600744"/>
+        <c:axId val="545599760"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="551222288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2050"/>
+          <c:min val="2010"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="551219664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="551219664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Years \</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Percent Efficiency</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="551222288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="545599760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Power Degradation Rate [%]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="545600744"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="545600744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="545599760"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="74000">
+              <a:schemeClr val="bg1">
+                <a:lumMod val="95000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="75000">
+              <a:schemeClr val="bg1"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="10800000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.52783370421639864"/>
+          <c:y val="0.64119463760934847"/>
+          <c:w val="0.3567983162288349"/>
+          <c:h val="0.25219681720719378"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200">
           <a:solidFill>
             <a:sysClr val="windowText" lastClr="000000"/>
           </a:solidFill>
@@ -26658,6 +28673,46 @@
 </file>
 
 <file path=xl/charts/colors16.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors17.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -30624,6 +32679,522 @@
 </file>
 
 <file path=xl/charts/style16.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style17.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -35878,6 +38449,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>142872</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>58736</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>536574</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1442BC87-28AF-4563-BE70-09874CD5CDB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -43357,7 +45969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886825C-AE4A-4EAF-970C-700F7CC3D78A}">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
@@ -47233,4 +49845,1273 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E72CE93-524C-4FA7-9EC7-337A4A16DA07}">
+  <dimension ref="A1:G58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V15" sqref="V15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1995</v>
+      </c>
+      <c r="B3">
+        <v>12.5</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>21</v>
+      </c>
+      <c r="E3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1996</v>
+      </c>
+      <c r="B4">
+        <v>12.7</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>21</v>
+      </c>
+      <c r="E4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>1997</v>
+      </c>
+      <c r="B5">
+        <v>12.88</v>
+      </c>
+      <c r="C5">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>23</v>
+      </c>
+      <c r="E5">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1998</v>
+      </c>
+      <c r="B6">
+        <v>13.06</v>
+      </c>
+      <c r="C6">
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <v>23</v>
+      </c>
+      <c r="E6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>1999</v>
+      </c>
+      <c r="B7">
+        <v>13.24</v>
+      </c>
+      <c r="C7">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>23</v>
+      </c>
+      <c r="E7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2000</v>
+      </c>
+      <c r="B8">
+        <v>13.42</v>
+      </c>
+      <c r="C8">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>23</v>
+      </c>
+      <c r="E8">
+        <v>0.6</v>
+      </c>
+      <c r="F8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>2001</v>
+      </c>
+      <c r="B9">
+        <v>13.6</v>
+      </c>
+      <c r="C9">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>23</v>
+      </c>
+      <c r="E9">
+        <v>0.6</v>
+      </c>
+      <c r="F9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>2002</v>
+      </c>
+      <c r="B10">
+        <v>13.722222220000001</v>
+      </c>
+      <c r="C10">
+        <v>19</v>
+      </c>
+      <c r="D10">
+        <v>23</v>
+      </c>
+      <c r="E10">
+        <v>0.6</v>
+      </c>
+      <c r="F10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2003</v>
+      </c>
+      <c r="B11">
+        <v>13.84444444</v>
+      </c>
+      <c r="C11">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>23</v>
+      </c>
+      <c r="E11">
+        <v>0.6</v>
+      </c>
+      <c r="F11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>2004</v>
+      </c>
+      <c r="B12">
+        <v>13.96666667</v>
+      </c>
+      <c r="C12">
+        <v>19</v>
+      </c>
+      <c r="D12">
+        <v>23</v>
+      </c>
+      <c r="E12">
+        <v>0.6</v>
+      </c>
+      <c r="F12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>2005</v>
+      </c>
+      <c r="B13">
+        <v>14.08888889</v>
+      </c>
+      <c r="C13">
+        <v>19</v>
+      </c>
+      <c r="D13">
+        <v>24</v>
+      </c>
+      <c r="E13">
+        <v>0.6</v>
+      </c>
+      <c r="F13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>2006</v>
+      </c>
+      <c r="B14">
+        <v>14.211111109999999</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
+      </c>
+      <c r="D14">
+        <v>25</v>
+      </c>
+      <c r="E14">
+        <v>0.6</v>
+      </c>
+      <c r="F14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>2007</v>
+      </c>
+      <c r="B15">
+        <v>14.33333333</v>
+      </c>
+      <c r="C15">
+        <v>20</v>
+      </c>
+      <c r="D15">
+        <v>25</v>
+      </c>
+      <c r="E15">
+        <v>0.6</v>
+      </c>
+      <c r="F15">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>2008</v>
+      </c>
+      <c r="B16">
+        <v>14.455555560000001</v>
+      </c>
+      <c r="C16">
+        <v>21</v>
+      </c>
+      <c r="D16">
+        <v>26</v>
+      </c>
+      <c r="E16">
+        <v>0.6</v>
+      </c>
+      <c r="F16">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>2009</v>
+      </c>
+      <c r="B17">
+        <v>14.57777778</v>
+      </c>
+      <c r="C17">
+        <v>24</v>
+      </c>
+      <c r="D17">
+        <v>29</v>
+      </c>
+      <c r="E17">
+        <v>0.6</v>
+      </c>
+      <c r="F17">
+        <v>21.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>2010</v>
+      </c>
+      <c r="B18">
+        <v>14.7</v>
+      </c>
+      <c r="C18">
+        <v>25</v>
+      </c>
+      <c r="D18">
+        <v>30</v>
+      </c>
+      <c r="E18">
+        <v>0.3</v>
+      </c>
+      <c r="F18">
+        <v>22.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>2011</v>
+      </c>
+      <c r="B19">
+        <v>15.1</v>
+      </c>
+      <c r="C19">
+        <v>25</v>
+      </c>
+      <c r="D19">
+        <v>30</v>
+      </c>
+      <c r="E19">
+        <v>0.3</v>
+      </c>
+      <c r="F19">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>2012</v>
+      </c>
+      <c r="B20">
+        <v>15.4</v>
+      </c>
+      <c r="C20">
+        <v>25</v>
+      </c>
+      <c r="D20">
+        <v>30</v>
+      </c>
+      <c r="E20">
+        <v>0.3</v>
+      </c>
+      <c r="F20">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>2013</v>
+      </c>
+      <c r="B21">
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <v>28</v>
+      </c>
+      <c r="D21">
+        <v>33</v>
+      </c>
+      <c r="E21">
+        <v>0.3</v>
+      </c>
+      <c r="F21">
+        <v>24.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>2014</v>
+      </c>
+      <c r="B22">
+        <v>16.3</v>
+      </c>
+      <c r="C22">
+        <v>28</v>
+      </c>
+      <c r="D22">
+        <v>33</v>
+      </c>
+      <c r="E22">
+        <v>0.3</v>
+      </c>
+      <c r="F22">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>2015</v>
+      </c>
+      <c r="B23">
+        <v>17</v>
+      </c>
+      <c r="C23">
+        <v>28</v>
+      </c>
+      <c r="D23">
+        <v>33</v>
+      </c>
+      <c r="E23">
+        <v>0.3</v>
+      </c>
+      <c r="F23">
+        <v>28.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>2016</v>
+      </c>
+      <c r="B24">
+        <v>17.5</v>
+      </c>
+      <c r="C24">
+        <v>28</v>
+      </c>
+      <c r="D24">
+        <v>33</v>
+      </c>
+      <c r="E24">
+        <v>0.3</v>
+      </c>
+      <c r="F24">
+        <v>28.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>2017</v>
+      </c>
+      <c r="B25">
+        <v>17.7</v>
+      </c>
+      <c r="C25">
+        <v>28</v>
+      </c>
+      <c r="D25">
+        <v>33</v>
+      </c>
+      <c r="E25">
+        <v>0.3</v>
+      </c>
+      <c r="F25">
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>2018</v>
+      </c>
+      <c r="B26">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="C26">
+        <v>28</v>
+      </c>
+      <c r="D26">
+        <v>33</v>
+      </c>
+      <c r="E26">
+        <v>0.3</v>
+      </c>
+      <c r="F26">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>2019</v>
+      </c>
+      <c r="B27">
+        <v>19.2</v>
+      </c>
+      <c r="C27">
+        <v>28</v>
+      </c>
+      <c r="D27">
+        <v>33</v>
+      </c>
+      <c r="E27">
+        <v>0.3</v>
+      </c>
+      <c r="F27">
+        <v>32.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>2020</v>
+      </c>
+      <c r="B28">
+        <v>20</v>
+      </c>
+      <c r="C28">
+        <v>33</v>
+      </c>
+      <c r="D28">
+        <v>38</v>
+      </c>
+      <c r="E28">
+        <v>0.5</v>
+      </c>
+      <c r="F28">
+        <v>35</v>
+      </c>
+      <c r="G28">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>2021</v>
+      </c>
+      <c r="B29">
+        <v>20.921698800000001</v>
+      </c>
+      <c r="C29">
+        <v>33</v>
+      </c>
+      <c r="D29">
+        <v>38</v>
+      </c>
+      <c r="E29">
+        <v>0.5</v>
+      </c>
+      <c r="F29">
+        <v>35</v>
+      </c>
+      <c r="G29">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>2022</v>
+      </c>
+      <c r="B30">
+        <v>21.480425369999999</v>
+      </c>
+      <c r="C30">
+        <v>33</v>
+      </c>
+      <c r="D30">
+        <v>38</v>
+      </c>
+      <c r="E30">
+        <v>0.5</v>
+      </c>
+      <c r="F30">
+        <v>35</v>
+      </c>
+      <c r="G30">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>2023</v>
+      </c>
+      <c r="B31">
+        <v>21.88587403</v>
+      </c>
+      <c r="C31">
+        <v>33</v>
+      </c>
+      <c r="D31">
+        <v>38</v>
+      </c>
+      <c r="E31">
+        <v>0.5</v>
+      </c>
+      <c r="F31">
+        <v>35</v>
+      </c>
+      <c r="G31">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>2024</v>
+      </c>
+      <c r="B32">
+        <v>22.205627280000002</v>
+      </c>
+      <c r="C32">
+        <v>33</v>
+      </c>
+      <c r="D32">
+        <v>38</v>
+      </c>
+      <c r="E32">
+        <v>0.5</v>
+      </c>
+      <c r="F32">
+        <v>35</v>
+      </c>
+      <c r="G32">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>2025</v>
+      </c>
+      <c r="B33">
+        <v>22.470349479999999</v>
+      </c>
+      <c r="C33">
+        <v>33</v>
+      </c>
+      <c r="D33">
+        <v>38</v>
+      </c>
+      <c r="E33">
+        <v>0.5</v>
+      </c>
+      <c r="F33">
+        <v>35</v>
+      </c>
+      <c r="G33">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>2026</v>
+      </c>
+      <c r="B34">
+        <v>22.6966295</v>
+      </c>
+      <c r="C34">
+        <v>33</v>
+      </c>
+      <c r="D34">
+        <v>38</v>
+      </c>
+      <c r="E34">
+        <v>0.5</v>
+      </c>
+      <c r="F34">
+        <v>35</v>
+      </c>
+      <c r="G34">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>2027</v>
+      </c>
+      <c r="B35">
+        <v>22.894483210000001</v>
+      </c>
+      <c r="C35">
+        <v>40</v>
+      </c>
+      <c r="D35">
+        <v>44</v>
+      </c>
+      <c r="E35">
+        <v>0.5</v>
+      </c>
+      <c r="F35">
+        <v>35</v>
+      </c>
+      <c r="G35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>2028</v>
+      </c>
+      <c r="B36">
+        <v>23.070433690000002</v>
+      </c>
+      <c r="C36">
+        <v>40</v>
+      </c>
+      <c r="D36">
+        <v>44</v>
+      </c>
+      <c r="E36">
+        <v>0.5</v>
+      </c>
+      <c r="F36">
+        <v>35</v>
+      </c>
+      <c r="G36">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>2029</v>
+      </c>
+      <c r="B37">
+        <v>23.228972280000001</v>
+      </c>
+      <c r="C37">
+        <v>40</v>
+      </c>
+      <c r="D37">
+        <v>44</v>
+      </c>
+      <c r="E37">
+        <v>0.5</v>
+      </c>
+      <c r="F37">
+        <v>35</v>
+      </c>
+      <c r="G37">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>2030</v>
+      </c>
+      <c r="B38">
+        <v>23.373326200000001</v>
+      </c>
+      <c r="C38">
+        <v>40</v>
+      </c>
+      <c r="D38">
+        <v>44</v>
+      </c>
+      <c r="E38">
+        <v>0.5</v>
+      </c>
+      <c r="F38">
+        <v>35</v>
+      </c>
+      <c r="G38">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>2031</v>
+      </c>
+      <c r="B39">
+        <v>23.505894179999999</v>
+      </c>
+      <c r="C39">
+        <v>40</v>
+      </c>
+      <c r="D39">
+        <v>44</v>
+      </c>
+      <c r="E39">
+        <v>0.5</v>
+      </c>
+      <c r="F39">
+        <v>35</v>
+      </c>
+      <c r="G39">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>2032</v>
+      </c>
+      <c r="B40">
+        <v>23.62850877</v>
+      </c>
+      <c r="C40">
+        <v>40</v>
+      </c>
+      <c r="D40">
+        <v>44</v>
+      </c>
+      <c r="E40">
+        <v>0.5</v>
+      </c>
+      <c r="F40">
+        <v>35</v>
+      </c>
+      <c r="G40">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>2033</v>
+      </c>
+      <c r="B41">
+        <v>23.742602300000001</v>
+      </c>
+      <c r="C41">
+        <v>40</v>
+      </c>
+      <c r="D41">
+        <v>44</v>
+      </c>
+      <c r="E41">
+        <v>0.5</v>
+      </c>
+      <c r="F41">
+        <v>35</v>
+      </c>
+      <c r="G41">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>2034</v>
+      </c>
+      <c r="B42">
+        <v>23.849315969999999</v>
+      </c>
+      <c r="C42">
+        <v>40</v>
+      </c>
+      <c r="D42">
+        <v>44</v>
+      </c>
+      <c r="E42">
+        <v>0.5</v>
+      </c>
+      <c r="F42">
+        <v>35</v>
+      </c>
+      <c r="G42">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>2035</v>
+      </c>
+      <c r="B43">
+        <v>23.949574089999999</v>
+      </c>
+      <c r="C43">
+        <v>40</v>
+      </c>
+      <c r="D43">
+        <v>44</v>
+      </c>
+      <c r="E43">
+        <v>0.5</v>
+      </c>
+      <c r="F43">
+        <v>35</v>
+      </c>
+      <c r="G43">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>2036</v>
+      </c>
+      <c r="B44">
+        <v>24.044135990000001</v>
+      </c>
+      <c r="C44">
+        <v>40</v>
+      </c>
+      <c r="D44">
+        <v>44</v>
+      </c>
+      <c r="E44">
+        <v>0.5</v>
+      </c>
+      <c r="F44">
+        <v>35</v>
+      </c>
+      <c r="G44">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>2037</v>
+      </c>
+      <c r="B45">
+        <v>24.133633240000002</v>
+      </c>
+      <c r="C45">
+        <v>40</v>
+      </c>
+      <c r="D45">
+        <v>44</v>
+      </c>
+      <c r="E45">
+        <v>0.5</v>
+      </c>
+      <c r="F45">
+        <v>35</v>
+      </c>
+      <c r="G45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>2038</v>
+      </c>
+      <c r="B46">
+        <v>24.218596949999998</v>
+      </c>
+      <c r="C46">
+        <v>40</v>
+      </c>
+      <c r="D46">
+        <v>44</v>
+      </c>
+      <c r="E46">
+        <v>0.5</v>
+      </c>
+      <c r="F46">
+        <v>35</v>
+      </c>
+      <c r="G46">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>2039</v>
+      </c>
+      <c r="B47">
+        <v>24.299478069999999</v>
+      </c>
+      <c r="C47">
+        <v>40</v>
+      </c>
+      <c r="D47">
+        <v>44</v>
+      </c>
+      <c r="E47">
+        <v>0.5</v>
+      </c>
+      <c r="F47">
+        <v>35</v>
+      </c>
+      <c r="G47">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>2040</v>
+      </c>
+      <c r="B48">
+        <v>24.376662799999998</v>
+      </c>
+      <c r="C48">
+        <v>40</v>
+      </c>
+      <c r="D48">
+        <v>44</v>
+      </c>
+      <c r="E48">
+        <v>0.5</v>
+      </c>
+      <c r="F48">
+        <v>35</v>
+      </c>
+      <c r="G48">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>2041</v>
+      </c>
+      <c r="B49">
+        <v>24.450484530000001</v>
+      </c>
+      <c r="C49">
+        <v>40</v>
+      </c>
+      <c r="D49">
+        <v>44</v>
+      </c>
+      <c r="E49">
+        <v>0.5</v>
+      </c>
+      <c r="F49">
+        <v>35</v>
+      </c>
+      <c r="G49">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>2042</v>
+      </c>
+      <c r="B50">
+        <v>24.52123306</v>
+      </c>
+      <c r="C50">
+        <v>40</v>
+      </c>
+      <c r="D50">
+        <v>44</v>
+      </c>
+      <c r="E50">
+        <v>0.5</v>
+      </c>
+      <c r="F50">
+        <v>35</v>
+      </c>
+      <c r="G50">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>2043</v>
+      </c>
+      <c r="B51">
+        <v>24.589161900000001</v>
+      </c>
+      <c r="C51">
+        <v>40</v>
+      </c>
+      <c r="D51">
+        <v>44</v>
+      </c>
+      <c r="E51">
+        <v>0.5</v>
+      </c>
+      <c r="F51">
+        <v>35</v>
+      </c>
+      <c r="G51">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>2044</v>
+      </c>
+      <c r="B52">
+        <v>24.654494150000001</v>
+      </c>
+      <c r="C52">
+        <v>40</v>
+      </c>
+      <c r="D52">
+        <v>44</v>
+      </c>
+      <c r="E52">
+        <v>0.5</v>
+      </c>
+      <c r="F52">
+        <v>35</v>
+      </c>
+      <c r="G52">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>2045</v>
+      </c>
+      <c r="B53">
+        <v>24.717427180000001</v>
+      </c>
+      <c r="C53">
+        <v>40</v>
+      </c>
+      <c r="D53">
+        <v>44</v>
+      </c>
+      <c r="E53">
+        <v>0.5</v>
+      </c>
+      <c r="F53">
+        <v>35</v>
+      </c>
+      <c r="G53">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>2046</v>
+      </c>
+      <c r="B54">
+        <v>24.778136459999999</v>
+      </c>
+      <c r="C54">
+        <v>40</v>
+      </c>
+      <c r="D54">
+        <v>44</v>
+      </c>
+      <c r="E54">
+        <v>0.5</v>
+      </c>
+      <c r="F54">
+        <v>35</v>
+      </c>
+      <c r="G54">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>2047</v>
+      </c>
+      <c r="B55">
+        <v>24.8367787</v>
+      </c>
+      <c r="C55">
+        <v>40</v>
+      </c>
+      <c r="D55">
+        <v>44</v>
+      </c>
+      <c r="E55">
+        <v>0.5</v>
+      </c>
+      <c r="F55">
+        <v>35</v>
+      </c>
+      <c r="G55">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>2048</v>
+      </c>
+      <c r="B56">
+        <v>24.893494459999999</v>
+      </c>
+      <c r="C56">
+        <v>40</v>
+      </c>
+      <c r="D56">
+        <v>44</v>
+      </c>
+      <c r="E56">
+        <v>0.5</v>
+      </c>
+      <c r="F56">
+        <v>35</v>
+      </c>
+      <c r="G56">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>2049</v>
+      </c>
+      <c r="B57">
+        <v>24.94841027</v>
+      </c>
+      <c r="C57">
+        <v>40</v>
+      </c>
+      <c r="D57">
+        <v>44</v>
+      </c>
+      <c r="E57">
+        <v>0.5</v>
+      </c>
+      <c r="F57">
+        <v>35</v>
+      </c>
+      <c r="G57">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>2050</v>
+      </c>
+      <c r="B58">
+        <v>25.001640479999999</v>
+      </c>
+      <c r="C58">
+        <v>40</v>
+      </c>
+      <c r="D58">
+        <v>44</v>
+      </c>
+      <c r="E58">
+        <v>0.5</v>
+      </c>
+      <c r="F58">
+        <v>35</v>
+      </c>
+      <c r="G58">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
figure tweaks for resubmission
getting dpi right
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/SupportingMaterial/BaselineGraphs.xlsx
+++ b/PV_ICE/baselines/SupportingMaterial/BaselineGraphs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFF3533-1044-47DA-9A33-78EC85D71F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BA104A-C648-4039-9CC4-A304B7711A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2340" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{31D47E9D-A833-4D35-B79A-EFF0E4DE6D01}"/>
+    <workbookView xWindow="-28920" yWindow="-2865" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{31D47E9D-A833-4D35-B79A-EFF0E4DE6D01}"/>
   </bookViews>
   <sheets>
     <sheet name="mass per m2" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,9 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -15052,6 +15055,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="545599760"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>

</xml_diff>